<commit_message>
Added govt in charge to layout
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39366\Desktop\Public_Debt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\39366\Desktop\PublicDebt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9491F0D-3133-4EDE-89E2-73BDEEB40A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64AEEE5C-2586-4327-9B2F-1A9902B94E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="866" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NOTE" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="306">
   <si>
     <t>Debito</t>
   </si>
@@ -728,6 +728,402 @@
   </si>
   <si>
     <t>FI</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_De_Gasperi_V</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Fanfani_V</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Moro_V</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Rumor_V</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Andreotti_V</t>
+  </si>
+  <si>
+    <t>Governo</t>
+  </si>
+  <si>
+    <t>Governo De Gasperi V</t>
+  </si>
+  <si>
+    <t>Governo De Gasperi VI</t>
+  </si>
+  <si>
+    <t>Governo Fanfani VI</t>
+  </si>
+  <si>
+    <t>Governo Andreotti VI</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_De_Gasperi_VI</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_De_Gasperi_VII</t>
+  </si>
+  <si>
+    <t>Governo De Gasperi VII</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_De_Gasperi_VIII</t>
+  </si>
+  <si>
+    <t>Governo De Gasperi VIII</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Pella</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Scelba</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Zoli</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Tambroni</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Colombo</t>
+  </si>
+  <si>
+    <t>Governo Pella</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Fanfani_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Segni_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Leone_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Moro_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Rumor_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Andreotti_I</t>
+  </si>
+  <si>
+    <t>Governo Fanfani I</t>
+  </si>
+  <si>
+    <t>Governo Scelba</t>
+  </si>
+  <si>
+    <t>Governo Segni I</t>
+  </si>
+  <si>
+    <t>Governo Leone I</t>
+  </si>
+  <si>
+    <t>Governo Moro I</t>
+  </si>
+  <si>
+    <t>Governo Rumor I</t>
+  </si>
+  <si>
+    <t>Governo Andreotti I</t>
+  </si>
+  <si>
+    <t>Governo Zoli</t>
+  </si>
+  <si>
+    <t>Governo Tambroni</t>
+  </si>
+  <si>
+    <t>Governo Colombo</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Fanfani_II</t>
+  </si>
+  <si>
+    <t>Governo Fanfani II</t>
+  </si>
+  <si>
+    <t>Governo Segni II</t>
+  </si>
+  <si>
+    <t>Governo Andreotti II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Segni_II</t>
+  </si>
+  <si>
+    <t>Governo Fanfani III</t>
+  </si>
+  <si>
+    <t>Governo Moro III</t>
+  </si>
+  <si>
+    <t>Governo Rumor III</t>
+  </si>
+  <si>
+    <t>Governo Andreotti III</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Fanfani_III</t>
+  </si>
+  <si>
+    <t>Governo Fanfani IV</t>
+  </si>
+  <si>
+    <t>Governo Moro IV</t>
+  </si>
+  <si>
+    <t>Governo Rumor IV</t>
+  </si>
+  <si>
+    <t>Governo Andreotti IV</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Fanfani_IV</t>
+  </si>
+  <si>
+    <t>Governo Moro II</t>
+  </si>
+  <si>
+    <t>Governo Leone II</t>
+  </si>
+  <si>
+    <t>Governo Rumor II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Moro_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Moro_III</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Leone_II</t>
+  </si>
+  <si>
+    <t>Governo Cossiga II</t>
+  </si>
+  <si>
+    <t>Governo Spadolini II</t>
+  </si>
+  <si>
+    <t>Governo Craxi II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Rumor_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Rumor_III</t>
+  </si>
+  <si>
+    <t>Governo Forlani</t>
+  </si>
+  <si>
+    <t>Governo Goria</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Andreotti_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Rumor_IV</t>
+  </si>
+  <si>
+    <t>Governo Rumor V</t>
+  </si>
+  <si>
+    <t>Governo Moro V</t>
+  </si>
+  <si>
+    <t>Governo Andreotti V</t>
+  </si>
+  <si>
+    <t>Governo Fanfani V</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Moro_IV</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Andreotti_IV</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Andreotti_III</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Berlusconi_III</t>
+  </si>
+  <si>
+    <t>Governo Berlusconi IV</t>
+  </si>
+  <si>
+    <t>Governo Cossiga I</t>
+  </si>
+  <si>
+    <t>Governo Spadolini I</t>
+  </si>
+  <si>
+    <t>Governo Craxi I</t>
+  </si>
+  <si>
+    <t>Governo Amato I</t>
+  </si>
+  <si>
+    <t>Governo Berlusconi I</t>
+  </si>
+  <si>
+    <t>Governo Prodi I</t>
+  </si>
+  <si>
+    <t>Governo D'Alema I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Cossiga_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Cossiga_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Spadolini_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Craxi_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Amato_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Berlusconi_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Prodi_II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Forlani</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Spadolini_I</t>
+  </si>
+  <si>
+    <t>PSI</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Craxi_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Fanfani_VI</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Goria</t>
+  </si>
+  <si>
+    <t>Governo De Mita</t>
+  </si>
+  <si>
+    <t>Governo Dini</t>
+  </si>
+  <si>
+    <t>Governo Monti</t>
+  </si>
+  <si>
+    <t>Governo Letta</t>
+  </si>
+  <si>
+    <t>Governo Renzi</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_De_Mita</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Andreotti_VI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://it.wikipedia.org/wiki/Governo_Andreotti_VII </t>
+  </si>
+  <si>
+    <t>Governo Andreotti VII</t>
+  </si>
+  <si>
+    <t>Governo Conte I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Amato_I</t>
+  </si>
+  <si>
+    <t>Governo Ciampi</t>
+  </si>
+  <si>
+    <t>Governo Draghi</t>
+  </si>
+  <si>
+    <t>Governo Meloni</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Ciampi</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Berlusconi_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Dini</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Prodi_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_D%27Alema_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_D%27Alema_II</t>
+  </si>
+  <si>
+    <t>Governo D'Alema II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Conte_II</t>
+  </si>
+  <si>
+    <t>Governo Amato II</t>
+  </si>
+  <si>
+    <t>Governo Berlusconi II</t>
+  </si>
+  <si>
+    <t>Governo Conte II</t>
+  </si>
+  <si>
+    <t>Governo Berlusconi III</t>
+  </si>
+  <si>
+    <t>Governo Prodi II</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Berlusconi_IV</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Monti</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Letta</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Renzi</t>
+  </si>
+  <si>
+    <t>Governo Gentiloni</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Gentiloni</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Conte_I</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Draghi</t>
+  </si>
+  <si>
+    <t>https://it.wikipedia.org/wiki/Governo_Meloni</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1730,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1358,6 +1753,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1398,27 +1814,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -1779,22 +2175,22 @@
       </c>
     </row>
     <row r="4" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="99" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="109" t="s">
+      <c r="C4" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="110" t="s">
+      <c r="D4" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="111" t="s">
+      <c r="E4" s="97" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="111" t="s">
+      <c r="F4" s="97" t="s">
         <v>89</v>
       </c>
-      <c r="G4" s="106" t="s">
+      <c r="G4" s="91" t="s">
         <v>90</v>
       </c>
       <c r="H4" s="77" t="s">
@@ -1802,33 +2198,33 @@
       </c>
     </row>
     <row r="5" spans="2:8" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="93"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="110"/>
-      <c r="E5" s="111"/>
-      <c r="F5" s="111"/>
-      <c r="G5" s="106"/>
+      <c r="B5" s="99"/>
+      <c r="C5" s="95"/>
+      <c r="D5" s="96"/>
+      <c r="E5" s="97"/>
+      <c r="F5" s="97"/>
+      <c r="G5" s="91"/>
       <c r="H5" s="77" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="E6" s="105" t="s">
+      <c r="E6" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="105" t="s">
+      <c r="F6" s="94" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="107" t="s">
+      <c r="G6" s="92" t="s">
         <v>91</v>
       </c>
       <c r="H6" s="5" t="s">
@@ -1836,12 +2232,12 @@
       </c>
     </row>
     <row r="7" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="94"/>
-      <c r="C7" s="103"/>
-      <c r="D7" s="104"/>
-      <c r="E7" s="105"/>
-      <c r="F7" s="105"/>
-      <c r="G7" s="107"/>
+      <c r="B7" s="100"/>
+      <c r="C7" s="109"/>
+      <c r="D7" s="110"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="92"/>
       <c r="H7" s="66" t="s">
         <v>55</v>
       </c>
@@ -1870,22 +2266,22 @@
       </c>
     </row>
     <row r="9" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="95" t="s">
+      <c r="C9" s="101" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="96" t="s">
+      <c r="D9" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="103" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="98" t="s">
+      <c r="F9" s="104" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="108" t="s">
+      <c r="G9" s="93" t="s">
         <v>48</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -1893,33 +2289,33 @@
       </c>
     </row>
     <row r="10" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="94"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="108"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="101"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="103"/>
+      <c r="G10" s="93"/>
       <c r="H10" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="93" t="s">
+      <c r="B11" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="99" t="s">
+      <c r="C11" s="105" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="100" t="s">
+      <c r="D11" s="106" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="101" t="s">
+      <c r="E11" s="107" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="102" t="s">
+      <c r="F11" s="108" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="92" t="s">
+      <c r="G11" s="98" t="s">
         <v>47</v>
       </c>
       <c r="H11" s="64" t="s">
@@ -1927,12 +2323,12 @@
       </c>
     </row>
     <row r="12" spans="2:8" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="93"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="102"/>
-      <c r="G12" s="92"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="106"/>
+      <c r="E12" s="107"/>
+      <c r="F12" s="108"/>
+      <c r="G12" s="98"/>
       <c r="H12" s="65" t="s">
         <v>21</v>
       </c>
@@ -1969,14 +2365,6 @@
     <row r="16" spans="2:8" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B9:B10"/>
@@ -1993,6 +2381,14 @@
     <mergeCell ref="C6:C7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="E6:E7"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H8" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -2014,7 +2410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:GN86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="FH2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2545,7 +2941,7 @@
     </row>
     <row r="2" spans="1:196" x14ac:dyDescent="0.3">
       <c r="A2" s="56"/>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="86" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="58" t="s">
@@ -3051,7 +3447,7 @@
       <c r="A3" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="87" t="s">
         <v>31</v>
       </c>
       <c r="C3" s="59" t="s">
@@ -3060,494 +3456,494 @@
       <c r="D3" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="84">
+      <c r="E3" s="83">
         <v>59292.079504686946</v>
       </c>
-      <c r="F3" s="84">
+      <c r="F3" s="83">
         <v>60471.502270845573</v>
       </c>
-      <c r="G3" s="84">
+      <c r="G3" s="83">
         <v>62343.995865598321</v>
       </c>
-      <c r="H3" s="84">
+      <c r="H3" s="83">
         <v>62899.211007408871</v>
       </c>
-      <c r="I3" s="84">
+      <c r="I3" s="83">
         <v>67207.724230113497</v>
       </c>
-      <c r="J3" s="84">
+      <c r="J3" s="83">
         <v>67631.473321100872</v>
       </c>
-      <c r="K3" s="84">
+      <c r="K3" s="83">
         <v>62332.117917562005</v>
       </c>
-      <c r="L3" s="84">
+      <c r="L3" s="83">
         <v>63739.325955818313</v>
       </c>
-      <c r="M3" s="84">
+      <c r="M3" s="83">
         <v>64842.442006205769</v>
       </c>
-      <c r="N3" s="84">
+      <c r="N3" s="83">
         <v>67016.777347957686</v>
       </c>
-      <c r="O3" s="84">
+      <c r="O3" s="83">
         <v>65934.46702647717</v>
       </c>
-      <c r="P3" s="84">
+      <c r="P3" s="83">
         <v>64886.854042423511</v>
       </c>
-      <c r="Q3" s="84">
+      <c r="Q3" s="83">
         <v>64923.410959482913</v>
       </c>
-      <c r="R3" s="84">
+      <c r="R3" s="83">
         <v>68642.401088267987</v>
       </c>
-      <c r="S3" s="84">
+      <c r="S3" s="83">
         <v>69207.437961928488</v>
       </c>
-      <c r="T3" s="84">
+      <c r="T3" s="83">
         <v>67895.09921184041</v>
       </c>
-      <c r="U3" s="84">
+      <c r="U3" s="83">
         <v>68934.696750765885</v>
       </c>
-      <c r="V3" s="84">
+      <c r="V3" s="83">
         <v>71159.724030646074</v>
       </c>
-      <c r="W3" s="84">
+      <c r="W3" s="83">
         <v>71768.929536357216</v>
       </c>
-      <c r="X3" s="84">
+      <c r="X3" s="83">
         <v>73346.849483739701</v>
       </c>
-      <c r="Y3" s="84">
+      <c r="Y3" s="83">
         <v>75651.865010252208</v>
       </c>
-      <c r="Z3" s="84">
+      <c r="Z3" s="83">
         <v>77197.241141206803</v>
       </c>
-      <c r="AA3" s="84">
+      <c r="AA3" s="83">
         <v>78459.078729729939</v>
       </c>
-      <c r="AB3" s="84">
+      <c r="AB3" s="83">
         <v>77834.56910666576</v>
       </c>
-      <c r="AC3" s="84">
+      <c r="AC3" s="83">
         <v>79730.898508639584</v>
       </c>
-      <c r="AD3" s="84">
+      <c r="AD3" s="83">
         <v>82160.524476683364</v>
       </c>
-      <c r="AE3" s="84">
+      <c r="AE3" s="83">
         <v>84713.097239643859</v>
       </c>
-      <c r="AF3" s="84">
+      <c r="AF3" s="83">
         <v>84874.656544060505</v>
       </c>
-      <c r="AG3" s="84">
+      <c r="AG3" s="83">
         <v>82725.01349036477</v>
       </c>
-      <c r="AH3" s="84">
+      <c r="AH3" s="83">
         <v>83530.906472329967</v>
       </c>
-      <c r="AI3" s="84">
+      <c r="AI3" s="83">
         <v>85129.570993138856</v>
       </c>
-      <c r="AJ3" s="84">
+      <c r="AJ3" s="83">
         <v>85761.935542106832</v>
       </c>
-      <c r="AK3" s="84">
+      <c r="AK3" s="83">
         <v>87654.502127502055</v>
       </c>
-      <c r="AL3" s="84">
+      <c r="AL3" s="83">
         <v>88765.64117183628</v>
       </c>
-      <c r="AM3" s="84">
+      <c r="AM3" s="83">
         <v>90003.068511745048</v>
       </c>
-      <c r="AN3" s="84">
+      <c r="AN3" s="83">
         <v>91805.561265938624</v>
       </c>
-      <c r="AO3" s="84">
+      <c r="AO3" s="83">
         <v>92478.497920559399</v>
       </c>
-      <c r="AP3" s="84">
+      <c r="AP3" s="83">
         <v>92795.796917697939</v>
       </c>
-      <c r="AQ3" s="84">
+      <c r="AQ3" s="83">
         <v>94299.462595087738</v>
       </c>
-      <c r="AR3" s="84">
+      <c r="AR3" s="83">
         <v>97472.325408755118</v>
       </c>
-      <c r="AS3" s="84">
+      <c r="AS3" s="83">
         <v>99470.588121539244</v>
       </c>
-      <c r="AT3" s="84">
+      <c r="AT3" s="83">
         <v>101872.1161030514</v>
       </c>
-      <c r="AU3" s="84">
+      <c r="AU3" s="83">
         <v>103708.36844168669</v>
       </c>
-      <c r="AV3" s="84">
+      <c r="AV3" s="83">
         <v>106258.06252464432</v>
       </c>
-      <c r="AW3" s="84">
+      <c r="AW3" s="83">
         <v>109442.5682472654</v>
       </c>
-      <c r="AX3" s="84">
+      <c r="AX3" s="83">
         <v>114035.24700782413</v>
       </c>
-      <c r="AY3" s="84">
+      <c r="AY3" s="83">
         <v>117048.51988031453</v>
       </c>
-      <c r="AZ3" s="84">
+      <c r="AZ3" s="83">
         <v>120528.771934358</v>
       </c>
-      <c r="BA3" s="84">
+      <c r="BA3" s="83">
         <v>122554.48857501365</v>
       </c>
-      <c r="BB3" s="84">
+      <c r="BB3" s="83">
         <v>123732.2868733846</v>
       </c>
-      <c r="BC3" s="84">
+      <c r="BC3" s="83">
         <v>126473.50914492289</v>
       </c>
-      <c r="BD3" s="84">
+      <c r="BD3" s="83">
         <v>127581.94659895834</v>
       </c>
-      <c r="BE3" s="84">
+      <c r="BE3" s="83">
         <v>134228.19055537856</v>
       </c>
-      <c r="BF3" s="84">
+      <c r="BF3" s="83">
         <v>126959.14680642834</v>
       </c>
-      <c r="BG3" s="84">
+      <c r="BG3" s="83">
         <v>122338.21387843326</v>
       </c>
-      <c r="BH3" s="84">
+      <c r="BH3" s="83">
         <v>133710.17778889253</v>
       </c>
-      <c r="BI3" s="84">
+      <c r="BI3" s="83">
         <v>133963.62972998302</v>
       </c>
-      <c r="BJ3" s="84">
+      <c r="BJ3" s="83">
         <v>129655.86585257592</v>
       </c>
-      <c r="BK3" s="84">
+      <c r="BK3" s="83">
         <v>122327.5324347523</v>
       </c>
-      <c r="BL3" s="84">
+      <c r="BL3" s="83">
         <v>125611.55763279818</v>
       </c>
-      <c r="BM3" s="84">
+      <c r="BM3" s="83">
         <v>121940.42169046534</v>
       </c>
-      <c r="BN3" s="84">
+      <c r="BN3" s="83">
         <v>132237.0633428052</v>
       </c>
-      <c r="BO3" s="84">
+      <c r="BO3" s="83">
         <v>144529.62680736402</v>
       </c>
-      <c r="BP3" s="84">
+      <c r="BP3" s="83">
         <v>148452.88424130465</v>
       </c>
-      <c r="BQ3" s="84">
+      <c r="BQ3" s="83">
         <v>158695.24161637158</v>
       </c>
-      <c r="BR3" s="84">
+      <c r="BR3" s="83">
         <v>159982.87554756601</v>
       </c>
-      <c r="BS3" s="84">
+      <c r="BS3" s="83">
         <v>157015.05269823069</v>
       </c>
-      <c r="BT3" s="84">
+      <c r="BT3" s="83">
         <v>166944.85697035576</v>
       </c>
-      <c r="BU3" s="84">
+      <c r="BU3" s="83">
         <v>175291.16613463862</v>
       </c>
-      <c r="BV3" s="84">
+      <c r="BV3" s="83">
         <v>167067.11204113075</v>
       </c>
-      <c r="BW3" s="84">
+      <c r="BW3" s="83">
         <v>165348.47104619327</v>
       </c>
-      <c r="BX3" s="84">
+      <c r="BX3" s="83">
         <v>168864.74265719898</v>
       </c>
-      <c r="BY3" s="84">
+      <c r="BY3" s="83">
         <v>166869.63505547572</v>
       </c>
-      <c r="BZ3" s="84">
+      <c r="BZ3" s="83">
         <v>166439.87206126878</v>
       </c>
-      <c r="CA3" s="84">
+      <c r="CA3" s="83">
         <v>175479.3002301025</v>
       </c>
-      <c r="CB3" s="84">
+      <c r="CB3" s="83">
         <v>169246.33914726888</v>
       </c>
-      <c r="CC3" s="84">
+      <c r="CC3" s="83">
         <v>186067.02780882141</v>
       </c>
-      <c r="CD3" s="84">
+      <c r="CD3" s="83">
         <v>191379.3352881856</v>
       </c>
-      <c r="CE3" s="84">
+      <c r="CE3" s="83">
         <v>203355.45517495091</v>
       </c>
-      <c r="CF3" s="84">
+      <c r="CF3" s="83">
         <v>199938.99281103746</v>
       </c>
-      <c r="CG3" s="84">
+      <c r="CG3" s="83">
         <v>196730.13732533582</v>
       </c>
-      <c r="CH3" s="84">
+      <c r="CH3" s="83">
         <v>185935.07473003573</v>
       </c>
-      <c r="CI3" s="84">
+      <c r="CI3" s="83">
         <v>157645.46780990032</v>
       </c>
-      <c r="CJ3" s="84">
+      <c r="CJ3" s="83">
         <v>127142.55044373595</v>
       </c>
-      <c r="CK3" s="84">
+      <c r="CK3" s="83">
         <v>114087.96754168526</v>
       </c>
-      <c r="CL3" s="84">
+      <c r="CL3" s="83">
         <v>153886.4288095363</v>
       </c>
-      <c r="CM3" s="84">
+      <c r="CM3" s="83">
         <v>183457.91740548422</v>
       </c>
-      <c r="CN3" s="84">
+      <c r="CN3" s="83">
         <v>197642.23220606984</v>
       </c>
-      <c r="CO3" s="84">
+      <c r="CO3" s="83">
         <v>214618.25183925155</v>
       </c>
-      <c r="CP3" s="84">
+      <c r="CP3" s="83">
         <v>232665.50418521502</v>
       </c>
-      <c r="CQ3" s="84">
+      <c r="CQ3" s="83">
         <v>255192.18378721934</v>
       </c>
-      <c r="CR3" s="84">
+      <c r="CR3" s="83">
         <v>267318.15862171625</v>
       </c>
-      <c r="CS3" s="84">
+      <c r="CS3" s="83">
         <v>286967.30457669578</v>
       </c>
-      <c r="CT3" s="84">
+      <c r="CT3" s="83">
         <v>297859.57260656013</v>
       </c>
-      <c r="CU3" s="84">
+      <c r="CU3" s="83">
         <v>318630.88459622482</v>
       </c>
-      <c r="CV3" s="84">
+      <c r="CV3" s="83">
         <v>334465.77398489765</v>
       </c>
-      <c r="CW3" s="84">
+      <c r="CW3" s="83">
         <v>353605.90313738713</v>
       </c>
-      <c r="CX3" s="84">
+      <c r="CX3" s="83">
         <v>374615.81020076555</v>
       </c>
-      <c r="CY3" s="84">
+      <c r="CY3" s="83">
         <v>401276.04709453596</v>
       </c>
-      <c r="CZ3" s="84">
+      <c r="CZ3" s="83">
         <v>432200.97465986712</v>
       </c>
-      <c r="DA3" s="84">
+      <c r="DA3" s="83">
         <v>468795.00402774883</v>
       </c>
-      <c r="DB3" s="84">
+      <c r="DB3" s="83">
         <v>501525.5969161652</v>
       </c>
-      <c r="DC3" s="84">
+      <c r="DC3" s="83">
         <v>532704.67150343442</v>
       </c>
-      <c r="DD3" s="84">
+      <c r="DD3" s="83">
         <v>553797.11078334227</v>
       </c>
-      <c r="DE3" s="84">
+      <c r="DE3" s="83">
         <v>579295.21139423724</v>
       </c>
-      <c r="DF3" s="84">
+      <c r="DF3" s="83">
         <v>618009.59502686874</v>
       </c>
-      <c r="DG3" s="84">
+      <c r="DG3" s="83">
         <v>665685.11399390514</v>
       </c>
-      <c r="DH3" s="84">
+      <c r="DH3" s="83">
         <v>714411.30888809916</v>
       </c>
-      <c r="DI3" s="84">
+      <c r="DI3" s="83">
         <v>761521.84675721778</v>
       </c>
-      <c r="DJ3" s="84">
+      <c r="DJ3" s="83">
         <v>807484.3648291399</v>
       </c>
-      <c r="DK3" s="84">
+      <c r="DK3" s="83">
         <v>820523.90561451425</v>
       </c>
-      <c r="DL3" s="84">
+      <c r="DL3" s="83">
         <v>848630.7572325794</v>
       </c>
-      <c r="DM3" s="84">
+      <c r="DM3" s="83">
         <v>905655.93124648521</v>
       </c>
-      <c r="DN3" s="84">
+      <c r="DN3" s="83">
         <v>951388.15422788041</v>
       </c>
-      <c r="DO3" s="84">
+      <c r="DO3" s="83">
         <v>928439.30349553912</v>
       </c>
-      <c r="DP3" s="84">
+      <c r="DP3" s="83">
         <v>990176.54339037498</v>
       </c>
-      <c r="DQ3" s="84">
+      <c r="DQ3" s="83">
         <v>1011850.8422308001</v>
       </c>
-      <c r="DR3" s="84">
+      <c r="DR3" s="83">
         <v>1041181.8230240227</v>
       </c>
-      <c r="DS3" s="84">
+      <c r="DS3" s="83">
         <v>1099054.0448271995</v>
       </c>
-      <c r="DT3" s="84">
+      <c r="DT3" s="83">
         <v>1133115.8056248282</v>
       </c>
-      <c r="DU3" s="84">
+      <c r="DU3" s="83">
         <v>1139424.3150390401</v>
       </c>
-      <c r="DV3" s="84">
+      <c r="DV3" s="83">
         <v>1141198.7982205802</v>
       </c>
-      <c r="DW3" s="84">
+      <c r="DW3" s="83">
         <v>1151755.5875616886</v>
       </c>
-      <c r="DX3" s="84">
+      <c r="DX3" s="83">
         <v>1186454.4871501669</v>
       </c>
-      <c r="DY3" s="84">
+      <c r="DY3" s="83">
         <v>1217551.5885527448</v>
       </c>
-      <c r="DZ3" s="84">
+      <c r="DZ3" s="83">
         <v>1250545.7276655089</v>
       </c>
-      <c r="EA3" s="84">
+      <c r="EA3" s="83">
         <v>1288899.7723438451</v>
       </c>
-      <c r="EB3" s="84">
+      <c r="EB3" s="83">
         <v>1340829.9258293263</v>
       </c>
-      <c r="EC3" s="84">
+      <c r="EC3" s="83">
         <v>1384439.026809419</v>
       </c>
-      <c r="ED3" s="84">
+      <c r="ED3" s="83">
         <v>1411884.8860018766</v>
       </c>
-      <c r="EE3" s="84">
+      <c r="EE3" s="83">
         <v>1432201.6639913537</v>
       </c>
-      <c r="EF3" s="84">
+      <c r="EF3" s="83">
         <v>1442554.3834257214</v>
       </c>
-      <c r="EG3" s="84">
+      <c r="EG3" s="83">
         <v>1430509.0039918118</v>
       </c>
-      <c r="EH3" s="84">
+      <c r="EH3" s="83">
         <v>1460181.4107342192</v>
       </c>
-      <c r="EI3" s="84">
+      <c r="EI3" s="83">
         <v>1499354.9</v>
       </c>
-      <c r="EJ3" s="84">
+      <c r="EJ3" s="83">
         <v>1518348.5</v>
       </c>
-      <c r="EK3" s="84">
+      <c r="EK3" s="83">
         <v>1546137.5</v>
       </c>
-      <c r="EL3" s="84">
+      <c r="EL3" s="83">
         <v>1574132.1</v>
       </c>
-      <c r="EM3" s="84">
+      <c r="EM3" s="83">
         <v>1599723.2</v>
       </c>
-      <c r="EN3" s="84">
+      <c r="EN3" s="83">
         <v>1660304</v>
       </c>
-      <c r="EO3" s="84">
+      <c r="EO3" s="83">
         <v>1692702.7</v>
       </c>
-      <c r="EP3" s="84">
+      <c r="EP3" s="83">
         <v>1697001.2</v>
       </c>
-      <c r="EQ3" s="84">
+      <c r="EQ3" s="83">
         <v>1699353.7</v>
       </c>
-      <c r="ER3" s="84">
+      <c r="ER3" s="83">
         <v>1723545.6000000001</v>
       </c>
-      <c r="ES3" s="84">
+      <c r="ES3" s="83">
         <v>1737641.6</v>
       </c>
-      <c r="ET3" s="84">
+      <c r="ET3" s="83">
         <v>1768756.5</v>
       </c>
-      <c r="EU3" s="84">
+      <c r="EU3" s="83">
         <v>1795059.2</v>
       </c>
-      <c r="EV3" s="84">
+      <c r="EV3" s="83">
         <v>1777790.5</v>
       </c>
-      <c r="EW3" s="84">
+      <c r="EW3" s="83">
         <v>1683906.5</v>
       </c>
-      <c r="EX3" s="84">
+      <c r="EX3" s="83">
         <v>1712756.8</v>
       </c>
-      <c r="EY3" s="84">
+      <c r="EY3" s="83">
         <v>1724871.7</v>
       </c>
-      <c r="EZ3" s="84">
+      <c r="EZ3" s="83">
         <v>1673454.9</v>
       </c>
-      <c r="FA3" s="84">
+      <c r="FA3" s="83">
         <v>1642645.5</v>
       </c>
-      <c r="FB3" s="84">
+      <c r="FB3" s="83">
         <v>1642570.8</v>
       </c>
-      <c r="FC3" s="84">
+      <c r="FC3" s="83">
         <v>1655355</v>
       </c>
-      <c r="FD3" s="84">
+      <c r="FD3" s="83">
         <v>1676766.4</v>
       </c>
-      <c r="FE3" s="84">
+      <c r="FE3" s="83">
         <v>1704732.5</v>
       </c>
-      <c r="FF3" s="84">
+      <c r="FF3" s="83">
         <v>1720826.7</v>
       </c>
-      <c r="FG3" s="85">
+      <c r="FG3" s="84">
         <v>1726724.3</v>
       </c>
-      <c r="FH3" s="91"/>
-      <c r="FI3" s="91"/>
-      <c r="FJ3" s="91"/>
-      <c r="FK3" s="91"/>
-      <c r="FL3" s="91"/>
+      <c r="FH3" s="90"/>
+      <c r="FI3" s="90"/>
+      <c r="FJ3" s="90"/>
+      <c r="FK3" s="90"/>
+      <c r="FL3" s="90"/>
     </row>
     <row r="4" spans="1:196" x14ac:dyDescent="0.3">
       <c r="A4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="87" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="59" t="s">
@@ -3556,496 +3952,496 @@
       <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="84">
+      <c r="E4" s="83">
         <v>4.4547341436454948</v>
       </c>
-      <c r="F4" s="84">
+      <c r="F4" s="83">
         <v>4.5081317079527397</v>
       </c>
-      <c r="G4" s="84">
+      <c r="G4" s="83">
         <v>4.4443384356131199</v>
       </c>
-      <c r="H4" s="84">
+      <c r="H4" s="83">
         <v>4.4537072039432539</v>
       </c>
-      <c r="I4" s="84">
+      <c r="I4" s="83">
         <v>4.7594584295538667</v>
       </c>
-      <c r="J4" s="84">
+      <c r="J4" s="83">
         <v>5.0696361043049363</v>
       </c>
-      <c r="K4" s="84">
+      <c r="K4" s="83">
         <v>4.8675644425902673</v>
       </c>
-      <c r="L4" s="84">
+      <c r="L4" s="83">
         <v>5.1348879821681015</v>
       </c>
-      <c r="M4" s="84">
+      <c r="M4" s="83">
         <v>4.9459409123067193</v>
       </c>
-      <c r="N4" s="84">
+      <c r="N4" s="83">
         <v>5.0563476724642689</v>
       </c>
-      <c r="O4" s="84">
+      <c r="O4" s="83">
         <v>5.0979632604389762</v>
       </c>
-      <c r="P4" s="84">
+      <c r="P4" s="83">
         <v>5.4482915828361609</v>
       </c>
-      <c r="Q4" s="84">
+      <c r="Q4" s="83">
         <v>6.0735931418516111</v>
       </c>
-      <c r="R4" s="84">
+      <c r="R4" s="83">
         <v>6.1868084081884778</v>
       </c>
-      <c r="S4" s="84">
+      <c r="S4" s="83">
         <v>5.3182491027580427</v>
       </c>
-      <c r="T4" s="84">
+      <c r="T4" s="83">
         <v>5.2354893568103051</v>
       </c>
-      <c r="U4" s="84">
+      <c r="U4" s="83">
         <v>5.8968553615829125</v>
       </c>
-      <c r="V4" s="84">
+      <c r="V4" s="83">
         <v>5.8683220093652411</v>
       </c>
-      <c r="W4" s="84">
+      <c r="W4" s="83">
         <v>5.6332666481631337</v>
       </c>
-      <c r="X4" s="84">
+      <c r="X4" s="83">
         <v>5.987584338327034</v>
       </c>
-      <c r="Y4" s="84">
+      <c r="Y4" s="83">
         <v>5.8976312111002178</v>
       </c>
-      <c r="Z4" s="84">
+      <c r="Z4" s="83">
         <v>6.0831914826676821</v>
       </c>
-      <c r="AA4" s="84">
+      <c r="AA4" s="83">
         <v>5.8380568410606832</v>
       </c>
-      <c r="AB4" s="84">
+      <c r="AB4" s="83">
         <v>5.6536589880852564</v>
       </c>
-      <c r="AC4" s="84">
+      <c r="AC4" s="83">
         <v>6.0491691654160826</v>
       </c>
-      <c r="AD4" s="84">
+      <c r="AD4" s="83">
         <v>6.3880579773726236</v>
       </c>
-      <c r="AE4" s="84">
+      <c r="AE4" s="83">
         <v>6.1656368244116129</v>
       </c>
-      <c r="AF4" s="84">
+      <c r="AF4" s="83">
         <v>6.1206015255068218</v>
       </c>
-      <c r="AG4" s="84">
+      <c r="AG4" s="83">
         <v>6.3713282909869076</v>
       </c>
-      <c r="AH4" s="84">
+      <c r="AH4" s="83">
         <v>6.6854901309055395</v>
       </c>
-      <c r="AI4" s="84">
+      <c r="AI4" s="83">
         <v>6.6914263580664466</v>
       </c>
-      <c r="AJ4" s="84">
+      <c r="AJ4" s="83">
         <v>6.2896821361574595</v>
       </c>
-      <c r="AK4" s="84">
+      <c r="AK4" s="83">
         <v>6.2282388712306531</v>
       </c>
-      <c r="AL4" s="84">
+      <c r="AL4" s="83">
         <v>6.1006162231693146</v>
       </c>
-      <c r="AM4" s="84">
+      <c r="AM4" s="83">
         <v>6.4682626551536249</v>
       </c>
-      <c r="AN4" s="84">
+      <c r="AN4" s="83">
         <v>6.5892307150448852</v>
       </c>
-      <c r="AO4" s="84">
+      <c r="AO4" s="83">
         <v>6.616885372453873</v>
       </c>
-      <c r="AP4" s="84">
+      <c r="AP4" s="83">
         <v>6.7563669971798426</v>
       </c>
-      <c r="AQ4" s="84">
+      <c r="AQ4" s="83">
         <v>7.0128309716440027</v>
       </c>
-      <c r="AR4" s="84">
+      <c r="AR4" s="83">
         <v>7.1892137276733674</v>
       </c>
-      <c r="AS4" s="84">
+      <c r="AS4" s="83">
         <v>7.3477239892031241</v>
       </c>
-      <c r="AT4" s="84">
+      <c r="AT4" s="83">
         <v>7.3884072690114131</v>
       </c>
-      <c r="AU4" s="84">
+      <c r="AU4" s="83">
         <v>7.7080499971815364</v>
       </c>
-      <c r="AV4" s="84">
+      <c r="AV4" s="83">
         <v>7.7868472149927443</v>
       </c>
-      <c r="AW4" s="84">
+      <c r="AW4" s="83">
         <v>8.17085721799479</v>
       </c>
-      <c r="AX4" s="84">
+      <c r="AX4" s="83">
         <v>8.96128890243582</v>
       </c>
-      <c r="AY4" s="84">
+      <c r="AY4" s="83">
         <v>9.6291967393463089</v>
       </c>
-      <c r="AZ4" s="84">
+      <c r="AZ4" s="83">
         <v>9.5781839607383841</v>
       </c>
-      <c r="BA4" s="84">
+      <c r="BA4" s="83">
         <v>9.962994636422378</v>
       </c>
-      <c r="BB4" s="84">
+      <c r="BB4" s="83">
         <v>10.40986567274628</v>
       </c>
-      <c r="BC4" s="84">
+      <c r="BC4" s="83">
         <v>11.563359848912254</v>
       </c>
-      <c r="BD4" s="84">
+      <c r="BD4" s="83">
         <v>12.170277929709313</v>
       </c>
-      <c r="BE4" s="84">
+      <c r="BE4" s="83">
         <v>12.717299254088443</v>
       </c>
-      <c r="BF4" s="84">
+      <c r="BF4" s="83">
         <v>12.021405672433128</v>
       </c>
-      <c r="BG4" s="84">
+      <c r="BG4" s="83">
         <v>13.365664914109807</v>
       </c>
-      <c r="BH4" s="84">
+      <c r="BH4" s="83">
         <v>19.044612778126044</v>
       </c>
-      <c r="BI4" s="84">
+      <c r="BI4" s="83">
         <v>27.221088914176132</v>
       </c>
-      <c r="BJ4" s="84">
+      <c r="BJ4" s="83">
         <v>37.416601128604846</v>
       </c>
-      <c r="BK4" s="84">
+      <c r="BK4" s="83">
         <v>40.547449610880854</v>
       </c>
-      <c r="BL4" s="84">
+      <c r="BL4" s="83">
         <v>57.211064482393788</v>
       </c>
-      <c r="BM4" s="84">
+      <c r="BM4" s="83">
         <v>57.690416659701398</v>
       </c>
-      <c r="BN4" s="84">
+      <c r="BN4" s="83">
         <v>61.476063247208771</v>
       </c>
-      <c r="BO4" s="84">
+      <c r="BO4" s="83">
         <v>66.508415138529003</v>
       </c>
-      <c r="BP4" s="84">
+      <c r="BP4" s="83">
         <v>67.632068499921871</v>
       </c>
-      <c r="BQ4" s="84">
+      <c r="BQ4" s="83">
         <v>83.790106355658992</v>
       </c>
-      <c r="BR4" s="84">
+      <c r="BR4" s="83">
         <v>89.825761470218595</v>
       </c>
-      <c r="BS4" s="84">
+      <c r="BS4" s="83">
         <v>78.900410042425904</v>
       </c>
-      <c r="BT4" s="84">
+      <c r="BT4" s="83">
         <v>79.738056081950035</v>
       </c>
-      <c r="BU4" s="84">
+      <c r="BU4" s="83">
         <v>81.387784552289219</v>
       </c>
-      <c r="BV4" s="84">
+      <c r="BV4" s="83">
         <v>71.599132254641589</v>
       </c>
-      <c r="BW4" s="84">
+      <c r="BW4" s="83">
         <v>63.802794567857156</v>
       </c>
-      <c r="BX4" s="84">
+      <c r="BX4" s="83">
         <v>59.888832652330841</v>
       </c>
-      <c r="BY4" s="84">
+      <c r="BY4" s="83">
         <v>54.779314062680818</v>
       </c>
-      <c r="BZ4" s="84">
+      <c r="BZ4" s="83">
         <v>54.851935539097234</v>
       </c>
-      <c r="CA4" s="84">
+      <c r="CA4" s="83">
         <v>60.775106549353389</v>
       </c>
-      <c r="CB4" s="84">
+      <c r="CB4" s="83">
         <v>62.997432974118709</v>
       </c>
-      <c r="CC4" s="84">
+      <c r="CC4" s="83">
         <v>79.305813864672189</v>
       </c>
-      <c r="CD4" s="84">
+      <c r="CD4" s="83">
         <v>86.418445978201021</v>
       </c>
-      <c r="CE4" s="84">
+      <c r="CE4" s="83">
         <v>95.432221445317495</v>
       </c>
-      <c r="CF4" s="84">
+      <c r="CF4" s="83">
         <v>113.05539605286901</v>
       </c>
-      <c r="CG4" s="84">
+      <c r="CG4" s="83">
         <v>134.98835422096471</v>
       </c>
-      <c r="CH4" s="84">
+      <c r="CH4" s="83">
         <v>168.167763813996</v>
       </c>
-      <c r="CI4" s="84">
+      <c r="CI4" s="83">
         <v>229.27262212146414</v>
       </c>
-      <c r="CJ4" s="84">
+      <c r="CJ4" s="83">
         <v>448.59555124529618</v>
       </c>
-      <c r="CK4" s="84">
+      <c r="CK4" s="83">
         <v>831.90982897796459</v>
       </c>
-      <c r="CL4" s="84">
+      <c r="CL4" s="83">
         <v>1865.3759815122341</v>
       </c>
-      <c r="CM4" s="84">
+      <c r="CM4" s="83">
         <v>3608.5279879954442</v>
       </c>
-      <c r="CN4" s="84">
+      <c r="CN4" s="83">
         <v>4248.2886830986381</v>
       </c>
-      <c r="CO4" s="84">
+      <c r="CO4" s="83">
         <v>4489.2083326387637</v>
       </c>
-      <c r="CP4" s="84">
+      <c r="CP4" s="83">
         <v>5078.5225870808772</v>
       </c>
-      <c r="CQ4" s="84">
+      <c r="CQ4" s="83">
         <v>6030.9633568332847</v>
       </c>
-      <c r="CR4" s="84">
+      <c r="CR4" s="83">
         <v>6526.7954724387209</v>
       </c>
-      <c r="CS4" s="84">
+      <c r="CS4" s="83">
         <v>7251.392595077039</v>
       </c>
-      <c r="CT4" s="84">
+      <c r="CT4" s="83">
         <v>7752.7153837588348</v>
       </c>
-      <c r="CU4" s="84">
+      <c r="CU4" s="83">
         <v>8561.2350837319991</v>
       </c>
-      <c r="CV4" s="84">
+      <c r="CV4" s="83">
         <v>9350.9674947150397</v>
       </c>
-      <c r="CW4" s="84">
+      <c r="CW4" s="83">
         <v>10069.499270482624</v>
       </c>
-      <c r="CX4" s="84">
+      <c r="CX4" s="83">
         <v>10885.233132170539</v>
       </c>
-      <c r="CY4" s="84">
+      <c r="CY4" s="83">
         <v>11590.201772019136</v>
       </c>
-      <c r="CZ4" s="84">
+      <c r="CZ4" s="83">
         <v>12681.423808717318</v>
       </c>
-      <c r="DA4" s="84">
+      <c r="DA4" s="83">
         <v>14308.335069549532</v>
       </c>
-      <c r="DB4" s="84">
+      <c r="DB4" s="83">
         <v>16125.109449052907</v>
       </c>
-      <c r="DC4" s="84">
+      <c r="DC4" s="83">
         <v>18586.031828951167</v>
       </c>
-      <c r="DD4" s="84">
+      <c r="DD4" s="83">
         <v>20498.910376823667</v>
       </c>
-      <c r="DE4" s="84">
+      <c r="DE4" s="83">
         <v>22157.349012695802</v>
       </c>
-      <c r="DF4" s="84">
+      <c r="DF4" s="83">
         <v>24208.53181109771</v>
       </c>
-      <c r="DG4" s="84">
+      <c r="DG4" s="83">
         <v>26880.212728818984</v>
       </c>
-      <c r="DH4" s="84">
+      <c r="DH4" s="83">
         <v>29218.758060967335</v>
       </c>
-      <c r="DI4" s="84">
+      <c r="DI4" s="83">
         <v>32312.97861850759</v>
       </c>
-      <c r="DJ4" s="84">
+      <c r="DJ4" s="83">
         <v>36494.579142332019</v>
       </c>
-      <c r="DK4" s="84">
+      <c r="DK4" s="83">
         <v>39857.400750556146</v>
       </c>
-      <c r="DL4" s="84">
+      <c r="DL4" s="83">
         <v>43701.373382857149</v>
       </c>
-      <c r="DM4" s="84">
+      <c r="DM4" s="83">
         <v>52695.641002633027</v>
       </c>
-      <c r="DN4" s="84">
+      <c r="DN4" s="83">
         <v>66641.952036634495</v>
       </c>
-      <c r="DO4" s="84">
+      <c r="DO4" s="83">
         <v>76363.325715250641</v>
       </c>
-      <c r="DP4" s="84">
+      <c r="DP4" s="83">
         <v>95889.238319095923</v>
       </c>
-      <c r="DQ4" s="84">
+      <c r="DQ4" s="83">
         <v>116528.67948833948</v>
       </c>
-      <c r="DR4" s="84">
+      <c r="DR4" s="83">
         <v>137203.3730827593</v>
       </c>
-      <c r="DS4" s="84">
+      <c r="DS4" s="83">
         <v>167908.39418758659</v>
       </c>
-      <c r="DT4" s="84">
+      <c r="DT4" s="83">
         <v>209712.53664631143</v>
       </c>
-      <c r="DU4" s="84">
+      <c r="DU4" s="83">
         <v>251373.59390678644</v>
       </c>
-      <c r="DV4" s="84">
+      <c r="DV4" s="83">
         <v>296805.39127693267</v>
       </c>
-      <c r="DW4" s="84">
+      <c r="DW4" s="83">
         <v>345912.46804210736</v>
       </c>
-      <c r="DX4" s="84">
+      <c r="DX4" s="83">
         <v>395710.36026453169</v>
       </c>
-      <c r="DY4" s="84">
+      <c r="DY4" s="83">
         <v>444416.36685093818</v>
       </c>
-      <c r="DZ4" s="84">
+      <c r="DZ4" s="83">
         <v>492252.92077250482</v>
       </c>
-      <c r="EA4" s="84">
+      <c r="EA4" s="83">
         <v>539221.751447174</v>
       </c>
-      <c r="EB4" s="84">
+      <c r="EB4" s="83">
         <v>599903.21861626965</v>
       </c>
-      <c r="EC4" s="84">
+      <c r="EC4" s="83">
         <v>659194.24369060074</v>
       </c>
-      <c r="ED4" s="84">
+      <c r="ED4" s="83">
         <v>729200.37337214884</v>
       </c>
-      <c r="EE4" s="84">
+      <c r="EE4" s="83">
         <v>796796.54630388611</v>
       </c>
-      <c r="EF4" s="84">
+      <c r="EF4" s="83">
         <v>838973.43912074296</v>
       </c>
-      <c r="EG4" s="84">
+      <c r="EG4" s="83">
         <v>864810.45314710122</v>
       </c>
-      <c r="EH4" s="84">
+      <c r="EH4" s="83">
         <v>914919.22596628184</v>
       </c>
-      <c r="EI4" s="84">
+      <c r="EI4" s="83">
         <v>988243.2</v>
       </c>
-      <c r="EJ4" s="84">
+      <c r="EJ4" s="83">
         <v>1045872.7</v>
       </c>
-      <c r="EK4" s="84">
+      <c r="EK4" s="83">
         <v>1092357.3</v>
       </c>
-      <c r="EL4" s="84">
+      <c r="EL4" s="83">
         <v>1138856.1000000001</v>
       </c>
-      <c r="EM4" s="84">
+      <c r="EM4" s="83">
         <v>1175149.5</v>
       </c>
-      <c r="EN4" s="84">
+      <c r="EN4" s="83">
         <v>1241512.8999999999</v>
       </c>
-      <c r="EO4" s="84">
+      <c r="EO4" s="83">
         <v>1304136.8</v>
       </c>
-      <c r="EP4" s="84">
+      <c r="EP4" s="83">
         <v>1350258.9</v>
       </c>
-      <c r="EQ4" s="84">
+      <c r="EQ4" s="83">
         <v>1394693.2</v>
       </c>
-      <c r="ER4" s="84">
+      <c r="ER4" s="83">
         <v>1452319</v>
       </c>
-      <c r="ES4" s="84">
+      <c r="ES4" s="83">
         <v>1493635.3</v>
       </c>
-      <c r="ET4" s="84">
+      <c r="ET4" s="83">
         <v>1552686.8</v>
       </c>
-      <c r="EU4" s="84">
+      <c r="EU4" s="83">
         <v>1614839.8</v>
       </c>
-      <c r="EV4" s="84">
+      <c r="EV4" s="83">
         <v>1637699.4</v>
       </c>
-      <c r="EW4" s="84">
+      <c r="EW4" s="83">
         <v>1577255.9</v>
       </c>
-      <c r="EX4" s="84">
+      <c r="EX4" s="83">
         <v>1611279.4</v>
       </c>
-      <c r="EY4" s="84">
+      <c r="EY4" s="83">
         <v>1648755.8</v>
       </c>
-      <c r="EZ4" s="84">
+      <c r="EZ4" s="83">
         <v>1624358.7</v>
       </c>
-      <c r="FA4" s="84">
+      <c r="FA4" s="83">
         <v>1612751.3</v>
       </c>
-      <c r="FB4" s="84">
+      <c r="FB4" s="83">
         <v>1627405.6</v>
       </c>
-      <c r="FC4" s="84">
+      <c r="FC4" s="83">
         <v>1655355</v>
       </c>
-      <c r="FD4" s="84">
+      <c r="FD4" s="83">
         <v>1695786.8</v>
       </c>
-      <c r="FE4" s="84">
+      <c r="FE4" s="83">
         <v>1736592.8</v>
       </c>
-      <c r="FF4" s="84">
+      <c r="FF4" s="83">
         <v>1766168.2</v>
       </c>
-      <c r="FG4" s="85">
+      <c r="FG4" s="84">
         <v>1789747</v>
       </c>
-      <c r="FH4" s="85">
+      <c r="FH4" s="84">
         <v>1573680</v>
       </c>
-      <c r="FI4" s="85">
+      <c r="FI4" s="84">
         <v>1704457</v>
       </c>
-      <c r="FJ4" s="85">
+      <c r="FJ4" s="84">
         <v>1772395</v>
       </c>
-      <c r="FK4" s="85">
+      <c r="FK4" s="84">
         <v>1788713</v>
       </c>
-      <c r="FL4" s="85">
+      <c r="FL4" s="84">
         <v>1805464</v>
       </c>
     </row>
@@ -4053,7 +4449,7 @@
       <c r="A5" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="88" t="s">
+      <c r="B5" s="87" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="59" t="s">
@@ -4062,496 +4458,496 @@
       <c r="D5" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="84">
+      <c r="E5" s="83">
         <v>1.7</v>
       </c>
-      <c r="F5" s="84">
+      <c r="F5" s="83">
         <v>1.8</v>
       </c>
-      <c r="G5" s="84">
+      <c r="G5" s="83">
         <v>2.1</v>
       </c>
-      <c r="H5" s="84">
+      <c r="H5" s="83">
         <v>2.6</v>
       </c>
-      <c r="I5" s="84">
+      <c r="I5" s="83">
         <v>3</v>
       </c>
-      <c r="J5" s="84">
+      <c r="J5" s="83">
         <v>3.4</v>
       </c>
-      <c r="K5" s="84">
+      <c r="K5" s="83">
         <v>4</v>
       </c>
-      <c r="L5" s="84">
+      <c r="L5" s="83">
         <v>4.2</v>
       </c>
-      <c r="M5" s="84">
+      <c r="M5" s="83">
         <v>4.3</v>
       </c>
-      <c r="N5" s="84">
+      <c r="N5" s="83">
         <v>4.7</v>
       </c>
-      <c r="O5" s="84">
+      <c r="O5" s="83">
         <v>4.9000000000000004</v>
       </c>
-      <c r="P5" s="84">
+      <c r="P5" s="83">
         <v>5</v>
       </c>
-      <c r="Q5" s="84">
+      <c r="Q5" s="83">
         <v>5.0999999999999996</v>
       </c>
-      <c r="R5" s="84">
+      <c r="R5" s="83">
         <v>4.8</v>
       </c>
-      <c r="S5" s="84">
+      <c r="S5" s="83">
         <v>4.8</v>
       </c>
-      <c r="T5" s="84">
+      <c r="T5" s="83">
         <v>5.5</v>
       </c>
-      <c r="U5" s="84">
+      <c r="U5" s="83">
         <v>5.6</v>
       </c>
-      <c r="V5" s="84">
+      <c r="V5" s="83">
         <v>5.6</v>
       </c>
-      <c r="W5" s="84">
+      <c r="W5" s="83">
         <v>5.6</v>
       </c>
-      <c r="X5" s="84">
+      <c r="X5" s="83">
         <v>5.5</v>
       </c>
-      <c r="Y5" s="84">
+      <c r="Y5" s="83">
         <v>6.1</v>
       </c>
-      <c r="Z5" s="84">
+      <c r="Z5" s="83">
         <v>6.6</v>
       </c>
-      <c r="AA5" s="84">
+      <c r="AA5" s="83">
         <v>6.5</v>
       </c>
-      <c r="AB5" s="84">
+      <c r="AB5" s="83">
         <v>6.5</v>
       </c>
-      <c r="AC5" s="84">
+      <c r="AC5" s="83">
         <v>6.4</v>
       </c>
-      <c r="AD5" s="84">
+      <c r="AD5" s="83">
         <v>6.5</v>
       </c>
-      <c r="AE5" s="84">
+      <c r="AE5" s="83">
         <v>6.6</v>
       </c>
-      <c r="AF5" s="84">
+      <c r="AF5" s="83">
         <v>6.8</v>
       </c>
-      <c r="AG5" s="84">
+      <c r="AG5" s="83">
         <v>7</v>
       </c>
-      <c r="AH5" s="84">
+      <c r="AH5" s="83">
         <v>7</v>
       </c>
-      <c r="AI5" s="84">
+      <c r="AI5" s="83">
         <v>7.2</v>
       </c>
-      <c r="AJ5" s="84">
+      <c r="AJ5" s="83">
         <v>7.3</v>
       </c>
-      <c r="AK5" s="84">
+      <c r="AK5" s="83">
         <v>7.3</v>
       </c>
-      <c r="AL5" s="84">
+      <c r="AL5" s="83">
         <v>7.6</v>
       </c>
-      <c r="AM5" s="84">
+      <c r="AM5" s="83">
         <v>7.6</v>
       </c>
-      <c r="AN5" s="84">
+      <c r="AN5" s="83">
         <v>7.8</v>
       </c>
-      <c r="AO5" s="84">
+      <c r="AO5" s="83">
         <v>7.9</v>
       </c>
-      <c r="AP5" s="84">
+      <c r="AP5" s="83">
         <v>8</v>
       </c>
-      <c r="AQ5" s="84">
+      <c r="AQ5" s="83">
         <v>8</v>
       </c>
-      <c r="AR5" s="84">
+      <c r="AR5" s="83">
         <v>8</v>
       </c>
-      <c r="AS5" s="84">
+      <c r="AS5" s="83">
         <v>7.9</v>
       </c>
-      <c r="AT5" s="84">
+      <c r="AT5" s="83">
         <v>7.9</v>
       </c>
-      <c r="AU5" s="84">
+      <c r="AU5" s="83">
         <v>7.9</v>
       </c>
-      <c r="AV5" s="84">
+      <c r="AV5" s="83">
         <v>8</v>
       </c>
-      <c r="AW5" s="84">
+      <c r="AW5" s="83">
         <v>8.1</v>
       </c>
-      <c r="AX5" s="84">
+      <c r="AX5" s="83">
         <v>8.1</v>
       </c>
-      <c r="AY5" s="84">
+      <c r="AY5" s="83">
         <v>8.1999999999999993</v>
       </c>
-      <c r="AZ5" s="84">
+      <c r="AZ5" s="83">
         <v>8.4</v>
       </c>
-      <c r="BA5" s="84">
+      <c r="BA5" s="83">
         <v>8.5</v>
       </c>
-      <c r="BB5" s="84">
+      <c r="BB5" s="83">
         <v>8.6999999999999993</v>
       </c>
-      <c r="BC5" s="84">
+      <c r="BC5" s="83">
         <v>8.8000000000000007</v>
       </c>
-      <c r="BD5" s="84">
+      <c r="BD5" s="83">
         <v>9.1</v>
       </c>
-      <c r="BE5" s="84">
+      <c r="BE5" s="83">
         <v>9.4</v>
       </c>
-      <c r="BF5" s="84">
+      <c r="BF5" s="83">
         <v>10</v>
       </c>
-      <c r="BG5" s="84">
+      <c r="BG5" s="83">
         <v>12.6</v>
       </c>
-      <c r="BH5" s="84">
+      <c r="BH5" s="83">
         <v>15.9</v>
       </c>
-      <c r="BI5" s="84">
+      <c r="BI5" s="83">
         <v>26.6</v>
       </c>
-      <c r="BJ5" s="84">
+      <c r="BJ5" s="83">
         <v>36.200000000000003</v>
       </c>
-      <c r="BK5" s="84">
+      <c r="BK5" s="83">
         <v>56.4</v>
       </c>
-      <c r="BL5" s="84">
+      <c r="BL5" s="83">
         <v>90.9</v>
       </c>
-      <c r="BM5" s="84">
+      <c r="BM5" s="83">
         <v>91.4</v>
       </c>
-      <c r="BN5" s="84">
+      <c r="BN5" s="83">
         <v>90.9</v>
       </c>
-      <c r="BO5" s="84">
+      <c r="BO5" s="83">
         <v>98.9</v>
       </c>
-      <c r="BP5" s="84">
+      <c r="BP5" s="83">
         <v>103</v>
       </c>
-      <c r="BQ5" s="84">
+      <c r="BQ5" s="83">
         <v>92.9</v>
       </c>
-      <c r="BR5" s="84">
+      <c r="BR5" s="83">
         <v>84.9</v>
       </c>
-      <c r="BS5" s="84">
+      <c r="BS5" s="83">
         <v>84.4</v>
       </c>
-      <c r="BT5" s="84">
+      <c r="BT5" s="83">
         <v>82.8</v>
       </c>
-      <c r="BU5" s="84">
+      <c r="BU5" s="83">
         <v>83.1</v>
       </c>
-      <c r="BV5" s="84">
+      <c r="BV5" s="83">
         <v>83.3</v>
       </c>
-      <c r="BW5" s="84">
+      <c r="BW5" s="83">
         <v>72.2</v>
       </c>
-      <c r="BX5" s="84">
+      <c r="BX5" s="83">
         <v>55.7</v>
       </c>
-      <c r="BY5" s="84">
+      <c r="BY5" s="83">
         <v>57.2</v>
       </c>
-      <c r="BZ5" s="84">
+      <c r="BZ5" s="83">
         <v>60.2</v>
       </c>
-      <c r="CA5" s="84">
+      <c r="CA5" s="83">
         <v>61.1</v>
       </c>
-      <c r="CB5" s="84">
+      <c r="CB5" s="83">
         <v>66.599999999999994</v>
       </c>
-      <c r="CC5" s="84">
+      <c r="CC5" s="83">
         <v>70.2</v>
       </c>
-      <c r="CD5" s="84">
+      <c r="CD5" s="83">
         <v>75.400000000000006</v>
       </c>
-      <c r="CE5" s="84">
+      <c r="CE5" s="83">
         <v>81.7</v>
       </c>
-      <c r="CF5" s="84">
+      <c r="CF5" s="83">
         <v>99.6</v>
       </c>
-      <c r="CG5" s="84">
+      <c r="CG5" s="83">
         <v>140.69999999999999</v>
       </c>
-      <c r="CH5" s="84">
+      <c r="CH5" s="83">
         <v>194.9</v>
       </c>
-      <c r="CI5" s="84">
+      <c r="CI5" s="83">
         <v>262.60000000000002</v>
       </c>
-      <c r="CJ5" s="84">
+      <c r="CJ5" s="83">
         <v>397.8</v>
       </c>
-      <c r="CK5" s="84">
+      <c r="CK5" s="83">
         <v>574.1</v>
       </c>
-      <c r="CL5" s="84">
+      <c r="CL5" s="83">
         <v>752.8</v>
       </c>
-      <c r="CM5" s="84">
+      <c r="CM5" s="83">
         <v>926.4</v>
       </c>
-      <c r="CN5" s="84">
+      <c r="CN5" s="83">
         <v>1230.4000000000001</v>
       </c>
-      <c r="CO5" s="84">
+      <c r="CO5" s="83">
         <v>1445.6</v>
       </c>
-      <c r="CP5" s="84">
+      <c r="CP5" s="83">
         <v>1615.1</v>
       </c>
-      <c r="CQ5" s="84">
+      <c r="CQ5" s="83">
         <v>1907.1</v>
       </c>
-      <c r="CR5" s="84">
+      <c r="CR5" s="83">
         <v>2191.4</v>
       </c>
-      <c r="CS5" s="84">
+      <c r="CS5" s="83">
         <v>2492</v>
       </c>
-      <c r="CT5" s="84">
+      <c r="CT5" s="83">
         <v>2794.9</v>
       </c>
-      <c r="CU5" s="84">
+      <c r="CU5" s="83">
         <v>3078.4</v>
       </c>
-      <c r="CV5" s="84">
+      <c r="CV5" s="83">
         <v>3261.7</v>
       </c>
-      <c r="CW5" s="84">
+      <c r="CW5" s="83">
         <v>3440.6</v>
       </c>
-      <c r="CX5" s="84">
+      <c r="CX5" s="83">
         <v>3688.7</v>
       </c>
-      <c r="CY5" s="84">
+      <c r="CY5" s="83">
         <v>4056</v>
       </c>
-      <c r="CZ5" s="84">
+      <c r="CZ5" s="83">
         <v>4214.3</v>
       </c>
-      <c r="DA5" s="84">
+      <c r="DA5" s="83">
         <v>4485.5</v>
       </c>
-      <c r="DB5" s="84">
+      <c r="DB5" s="83">
         <v>4866.3999999999996</v>
       </c>
-      <c r="DC5" s="84">
+      <c r="DC5" s="83">
         <v>5235.1000000000004</v>
       </c>
-      <c r="DD5" s="84">
+      <c r="DD5" s="83">
         <v>5736.1</v>
       </c>
-      <c r="DE5" s="84">
+      <c r="DE5" s="83">
         <v>6434.2</v>
       </c>
-      <c r="DF5" s="84">
+      <c r="DF5" s="83">
         <v>8159.5</v>
       </c>
-      <c r="DG5" s="84">
+      <c r="DG5" s="83">
         <v>8939.7000000000007</v>
       </c>
-      <c r="DH5" s="84">
+      <c r="DH5" s="83">
         <v>10405.1</v>
       </c>
-      <c r="DI5" s="84">
+      <c r="DI5" s="83">
         <v>11690.8</v>
       </c>
-      <c r="DJ5" s="84">
+      <c r="DJ5" s="83">
         <v>13430.8</v>
       </c>
-      <c r="DK5" s="84">
+      <c r="DK5" s="83">
         <v>16445.8</v>
       </c>
-      <c r="DL5" s="84">
+      <c r="DL5" s="83">
         <v>20473.900000000001</v>
       </c>
-      <c r="DM5" s="84">
+      <c r="DM5" s="83">
         <v>26242.9</v>
       </c>
-      <c r="DN5" s="84">
+      <c r="DN5" s="83">
         <v>32941.5</v>
       </c>
-      <c r="DO5" s="84">
+      <c r="DO5" s="83">
         <v>42618.5</v>
       </c>
-      <c r="DP5" s="84">
+      <c r="DP5" s="83">
         <v>53193</v>
       </c>
-      <c r="DQ5" s="84">
+      <c r="DQ5" s="83">
         <v>63690.2</v>
       </c>
-      <c r="DR5" s="84">
+      <c r="DR5" s="83">
         <v>80760.2</v>
       </c>
-      <c r="DS5" s="84">
+      <c r="DS5" s="83">
         <v>96975.9</v>
       </c>
-      <c r="DT5" s="84">
+      <c r="DT5" s="83">
         <v>116744.8</v>
       </c>
-      <c r="DU5" s="84">
+      <c r="DU5" s="83">
         <v>145449.79999999999</v>
       </c>
-      <c r="DV5" s="84">
+      <c r="DV5" s="83">
         <v>185160.9</v>
       </c>
-      <c r="DW5" s="84">
+      <c r="DW5" s="83">
         <v>236605</v>
       </c>
-      <c r="DX5" s="84">
+      <c r="DX5" s="83">
         <v>291718.59999999998</v>
       </c>
-      <c r="DY5" s="84">
+      <c r="DY5" s="83">
         <v>354113.5</v>
       </c>
-      <c r="DZ5" s="84">
+      <c r="DZ5" s="83">
         <v>412760.1</v>
       </c>
-      <c r="EA5" s="84">
+      <c r="EA5" s="83">
         <v>473277.4</v>
       </c>
-      <c r="EB5" s="84">
+      <c r="EB5" s="83">
         <v>536865</v>
       </c>
-      <c r="EC5" s="84">
+      <c r="EC5" s="83">
         <v>606368.9</v>
       </c>
-      <c r="ED5" s="84">
+      <c r="ED5" s="83">
         <v>685300</v>
       </c>
-      <c r="EE5" s="84">
+      <c r="EE5" s="83">
         <v>774895.7</v>
       </c>
-      <c r="EF5" s="84">
+      <c r="EF5" s="83">
         <v>870995.5</v>
       </c>
-      <c r="EG5" s="84">
+      <c r="EG5" s="83">
         <v>983317.9</v>
       </c>
-      <c r="EH5" s="84">
+      <c r="EH5" s="83">
         <v>1094981.1000000001</v>
       </c>
-      <c r="EI5" s="84">
+      <c r="EI5" s="83">
         <v>1179588.7</v>
       </c>
-      <c r="EJ5" s="84">
+      <c r="EJ5" s="83">
         <v>1245731.3999999999</v>
       </c>
-      <c r="EK5" s="84">
+      <c r="EK5" s="83">
         <v>1275677.7</v>
       </c>
-      <c r="EL5" s="84">
+      <c r="EL5" s="83">
         <v>1299741.3</v>
       </c>
-      <c r="EM5" s="84">
+      <c r="EM5" s="83">
         <v>1331320.6000000001</v>
       </c>
-      <c r="EN5" s="84">
+      <c r="EN5" s="83">
         <v>1353569.3</v>
       </c>
-      <c r="EO5" s="84">
+      <c r="EO5" s="83">
         <v>1420027.8</v>
       </c>
-      <c r="EP5" s="84">
+      <c r="EP5" s="83">
         <v>1436141.8</v>
       </c>
-      <c r="EQ5" s="84">
+      <c r="EQ5" s="83">
         <v>1471325.7</v>
       </c>
-      <c r="ER5" s="84">
+      <c r="ER5" s="83">
         <v>1526400.5</v>
       </c>
-      <c r="ES5" s="84">
+      <c r="ES5" s="83">
         <v>1591580.6</v>
       </c>
-      <c r="ET5" s="84">
+      <c r="ET5" s="83">
         <v>1657334.2</v>
       </c>
-      <c r="EU5" s="84">
+      <c r="EU5" s="83">
         <v>1677649.8</v>
       </c>
-      <c r="EV5" s="84">
+      <c r="EV5" s="83">
         <v>1738647</v>
       </c>
-      <c r="EW5" s="84">
+      <c r="EW5" s="83">
         <v>1839232.6</v>
       </c>
-      <c r="EX5" s="84">
+      <c r="EX5" s="83">
         <v>1920615.2</v>
       </c>
-      <c r="EY5" s="86">
+      <c r="EY5" s="85">
         <v>1973433.2</v>
       </c>
-      <c r="EZ5" s="86">
+      <c r="EZ5" s="85">
         <v>2054702.9</v>
       </c>
-      <c r="FA5" s="84">
+      <c r="FA5" s="83">
         <v>2136175.6</v>
       </c>
-      <c r="FB5" s="84">
+      <c r="FB5" s="83">
         <v>2202946.6</v>
       </c>
-      <c r="FC5" s="84">
+      <c r="FC5" s="83">
         <v>2239359.2999999998</v>
       </c>
-      <c r="FD5" s="84">
+      <c r="FD5" s="83">
         <v>2285632.1</v>
       </c>
-      <c r="FE5" s="86">
+      <c r="FE5" s="85">
         <v>2329358.7000000002</v>
       </c>
-      <c r="FF5" s="84">
+      <c r="FF5" s="83">
         <v>2380947.2000000002</v>
       </c>
-      <c r="FG5" s="85">
+      <c r="FG5" s="84">
         <v>2409903.9</v>
       </c>
-      <c r="FH5" s="85">
+      <c r="FH5" s="84">
         <v>2409982</v>
       </c>
-      <c r="FI5" s="85">
+      <c r="FI5" s="84">
         <v>2573468</v>
       </c>
-      <c r="FJ5" s="85">
+      <c r="FJ5" s="84">
         <v>2758225</v>
       </c>
-      <c r="FK5" s="85">
+      <c r="FK5" s="84">
         <v>2863438</v>
       </c>
-      <c r="FL5" s="89">
+      <c r="FL5" s="88">
         <v>2948512</v>
       </c>
     </row>
@@ -6647,7 +7043,7 @@
       <c r="A9" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="88" t="s">
+      <c r="B9" s="87" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="59" t="s">
@@ -7131,19 +7527,19 @@
       <c r="FG9" s="45">
         <v>1.7732115209579902</v>
       </c>
-      <c r="FH9" s="90">
+      <c r="FH9" s="89">
         <v>1.77321152095799</v>
       </c>
-      <c r="FI9" s="90">
+      <c r="FI9" s="89">
         <v>1.7732115209579902</v>
       </c>
-      <c r="FJ9" s="90">
+      <c r="FJ9" s="89">
         <v>1.7732115209579902</v>
       </c>
-      <c r="FK9" s="90">
+      <c r="FK9" s="89">
         <v>1.7732115209579902</v>
       </c>
-      <c r="FL9" s="90">
+      <c r="FL9" s="89">
         <v>1.77321152095799</v>
       </c>
       <c r="FM9" s="15"/>
@@ -7873,7 +8269,7 @@
       <c r="A11" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="88" t="s">
+      <c r="B11" s="87" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="59" t="s">
@@ -16751,7 +17147,7 @@
       <c r="A24" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="87" t="s">
+      <c r="B24" s="86" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="60" t="s">
@@ -19296,23 +19692,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C936E7A-7728-4296-AA2C-EF23E41CBEE6}">
-  <dimension ref="A1:F66"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
     <col min="2" max="2" width="14.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="73.109375" customWidth="1"/>
-    <col min="6" max="6" width="14.21875" customWidth="1"/>
+    <col min="3" max="5" width="17.21875" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="73.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>97</v>
       </c>
@@ -19323,16 +19719,22 @@
         <v>99</v>
       </c>
       <c r="D1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>103</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="82">
         <v>17676</v>
       </c>
@@ -19342,17 +19744,23 @@
       <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" s="111" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>102</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="82">
         <v>18290</v>
       </c>
@@ -19362,17 +19770,23 @@
       <c r="C3" t="s">
         <v>101</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="111" t="s">
+        <v>184</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>104</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="82">
         <v>18835</v>
       </c>
@@ -19382,17 +19796,23 @@
       <c r="C4" t="s">
         <v>101</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E4" s="111" t="s">
+        <v>185</v>
+      </c>
+      <c r="F4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>105</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="82">
         <v>19556</v>
       </c>
@@ -19402,17 +19822,23 @@
       <c r="C5" t="s">
         <v>101</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E5" s="111" t="s">
+        <v>187</v>
+      </c>
+      <c r="F5">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>106</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="82">
         <v>19588</v>
       </c>
@@ -19422,17 +19848,23 @@
       <c r="C6" t="s">
         <v>107</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="111" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6">
         <v>2</v>
       </c>
-      <c r="E6" t="s">
+      <c r="G6" t="s">
         <v>134</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="82">
         <v>19742</v>
       </c>
@@ -19442,17 +19874,23 @@
       <c r="C7" t="s">
         <v>108</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="111" t="s">
+        <v>195</v>
+      </c>
+      <c r="F7">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>106</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="82">
         <v>19765</v>
       </c>
@@ -19462,17 +19900,23 @@
       <c r="C8" t="s">
         <v>109</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>202</v>
+      </c>
+      <c r="E8" s="111" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>110</v>
       </c>
-      <c r="F8" t="s">
+      <c r="H8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="82">
         <v>20276</v>
       </c>
@@ -19482,17 +19926,23 @@
       <c r="C9" t="s">
         <v>111</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E9" s="111" t="s">
+        <v>196</v>
+      </c>
+      <c r="F9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>110</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="82">
         <v>20959</v>
       </c>
@@ -19502,17 +19952,23 @@
       <c r="C10" t="s">
         <v>112</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>208</v>
+      </c>
+      <c r="E10" s="111" t="s">
+        <v>191</v>
+      </c>
+      <c r="F10">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>106</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="82">
         <v>21367</v>
       </c>
@@ -19522,17 +19978,23 @@
       <c r="C11" t="s">
         <v>108</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="111" t="s">
+        <v>211</v>
+      </c>
+      <c r="F11">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>113</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="82">
         <v>21597</v>
       </c>
@@ -19542,17 +20004,23 @@
       <c r="C12" t="s">
         <v>111</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>213</v>
+      </c>
+      <c r="E12" s="111" t="s">
+        <v>215</v>
+      </c>
+      <c r="F12">
         <v>3</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>106</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="82">
         <v>22000</v>
       </c>
@@ -19562,17 +20030,23 @@
       <c r="C13" t="s">
         <v>114</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>209</v>
+      </c>
+      <c r="E13" s="111" t="s">
+        <v>192</v>
+      </c>
+      <c r="F13">
         <v>3</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>106</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="82">
         <v>22123</v>
       </c>
@@ -19582,17 +20056,23 @@
       <c r="C14" t="s">
         <v>108</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="111" t="s">
+        <v>220</v>
+      </c>
+      <c r="F14">
         <v>3</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>106</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="82">
         <v>22698</v>
       </c>
@@ -19602,17 +20082,23 @@
       <c r="C15" t="s">
         <v>108</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="111" t="s">
+        <v>225</v>
+      </c>
+      <c r="F15">
         <v>3</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>115</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="82">
         <v>23183</v>
       </c>
@@ -19622,17 +20108,23 @@
       <c r="C16" t="s">
         <v>116</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>204</v>
+      </c>
+      <c r="E16" s="111" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16">
         <v>4</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>106</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="82">
         <v>23350</v>
       </c>
@@ -19642,17 +20134,23 @@
       <c r="C17" t="s">
         <v>117</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E17" s="111" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
+      <c r="G17" t="s">
         <v>118</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="82">
         <v>23580</v>
       </c>
@@ -19662,17 +20160,23 @@
       <c r="C18" t="s">
         <v>117</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>226</v>
+      </c>
+      <c r="E18" s="111" t="s">
+        <v>229</v>
+      </c>
+      <c r="F18">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>118</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="82">
         <v>24161</v>
       </c>
@@ -19682,17 +20186,23 @@
       <c r="C19" t="s">
         <v>117</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="s">
+        <v>217</v>
+      </c>
+      <c r="E19" s="111" t="s">
+        <v>230</v>
+      </c>
+      <c r="F19">
         <v>4</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>118</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="82">
         <v>25013</v>
       </c>
@@ -19702,17 +20212,23 @@
       <c r="C20" t="s">
         <v>116</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>227</v>
+      </c>
+      <c r="E20" s="111" t="s">
+        <v>231</v>
+      </c>
+      <c r="F20">
         <v>5</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>106</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="82">
         <v>25184</v>
       </c>
@@ -19722,17 +20238,23 @@
       <c r="C21" t="s">
         <v>119</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>206</v>
+      </c>
+      <c r="E21" s="111" t="s">
+        <v>199</v>
+      </c>
+      <c r="F21">
         <v>5</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>120</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="82">
         <v>25420</v>
       </c>
@@ -19742,17 +20264,23 @@
       <c r="C22" t="s">
         <v>119</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" s="111" t="s">
+        <v>235</v>
+      </c>
+      <c r="F22">
         <v>5</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>106</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="82">
         <v>25655</v>
       </c>
@@ -19762,17 +20290,23 @@
       <c r="C23" t="s">
         <v>119</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="s">
+        <v>218</v>
+      </c>
+      <c r="E23" s="111" t="s">
+        <v>236</v>
+      </c>
+      <c r="F23">
         <v>5</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>118</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="82">
         <v>25786</v>
       </c>
@@ -19782,17 +20316,23 @@
       <c r="C24" t="s">
         <v>121</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24" s="111" t="s">
+        <v>193</v>
+      </c>
+      <c r="F24">
         <v>5</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>118</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="82">
         <v>26346</v>
       </c>
@@ -19802,17 +20342,23 @@
       <c r="C25" t="s">
         <v>122</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E25" s="111" t="s">
+        <v>200</v>
+      </c>
+      <c r="F25">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>106</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="82">
         <v>26476</v>
       </c>
@@ -19822,17 +20368,23 @@
       <c r="C26" t="s">
         <v>122</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="111" t="s">
+        <v>239</v>
+      </c>
+      <c r="F26">
         <v>6</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>123</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="82">
         <v>26852</v>
       </c>
@@ -19842,17 +20394,23 @@
       <c r="C27" t="s">
         <v>119</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="s">
+        <v>223</v>
+      </c>
+      <c r="E27" s="111" t="s">
+        <v>240</v>
+      </c>
+      <c r="F27">
         <v>6</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>124</v>
       </c>
-      <c r="F27" t="s">
+      <c r="H27" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="82">
         <v>27102</v>
       </c>
@@ -19862,17 +20420,23 @@
       <c r="C28" t="s">
         <v>119</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="s">
+        <v>241</v>
+      </c>
+      <c r="E28" s="111" t="s">
+        <v>177</v>
+      </c>
+      <c r="F28">
         <v>6</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>125</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="82">
         <v>27356</v>
       </c>
@@ -19882,17 +20446,23 @@
       <c r="C29" t="s">
         <v>117</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="s">
+        <v>222</v>
+      </c>
+      <c r="E29" s="111" t="s">
+        <v>245</v>
+      </c>
+      <c r="F29">
         <v>6</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>105</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="82">
         <v>27802</v>
       </c>
@@ -19902,17 +20472,23 @@
       <c r="C30" t="s">
         <v>117</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="111" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30">
         <v>6</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>106</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="82">
         <v>27970</v>
       </c>
@@ -19922,17 +20498,23 @@
       <c r="C31" t="s">
         <v>122</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="s">
+        <v>219</v>
+      </c>
+      <c r="E31" s="111" t="s">
+        <v>247</v>
+      </c>
+      <c r="F31">
         <v>7</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>106</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="82">
         <v>28560</v>
       </c>
@@ -19942,17 +20524,23 @@
       <c r="C32" t="s">
         <v>122</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="s">
+        <v>224</v>
+      </c>
+      <c r="E32" s="111" t="s">
+        <v>246</v>
+      </c>
+      <c r="F32">
         <v>7</v>
       </c>
-      <c r="E32" t="s">
+      <c r="G32" t="s">
         <v>106</v>
       </c>
-      <c r="F32" t="s">
+      <c r="H32" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="82">
         <v>28934</v>
       </c>
@@ -19962,17 +20550,23 @@
       <c r="C33" t="s">
         <v>122</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="s">
+        <v>243</v>
+      </c>
+      <c r="E33" s="111" t="s">
+        <v>178</v>
+      </c>
+      <c r="F33">
         <v>7</v>
       </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>115</v>
       </c>
-      <c r="F33" t="s">
+      <c r="H33" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="82">
         <v>29315</v>
       </c>
@@ -19982,17 +20576,23 @@
       <c r="C34" t="s">
         <v>126</v>
       </c>
-      <c r="D34">
+      <c r="D34" t="s">
+        <v>250</v>
+      </c>
+      <c r="E34" s="111" t="s">
+        <v>257</v>
+      </c>
+      <c r="F34">
         <v>8</v>
       </c>
-      <c r="E34" t="s">
+      <c r="G34" t="s">
         <v>120</v>
       </c>
-      <c r="F34" t="s">
+      <c r="H34" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="82">
         <v>29072</v>
       </c>
@@ -20002,17 +20602,23 @@
       <c r="C35" t="s">
         <v>126</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="s">
+        <v>232</v>
+      </c>
+      <c r="E35" s="111" t="s">
+        <v>258</v>
+      </c>
+      <c r="F35">
         <v>8</v>
       </c>
-      <c r="E35" t="s">
+      <c r="G35" t="s">
         <v>110</v>
       </c>
-      <c r="F35" t="s">
+      <c r="H35" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="82">
         <v>29512</v>
       </c>
@@ -20022,17 +20628,23 @@
       <c r="C36" t="s">
         <v>127</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="s">
+        <v>237</v>
+      </c>
+      <c r="E36" s="111" t="s">
+        <v>264</v>
+      </c>
+      <c r="F36">
         <v>8</v>
       </c>
-      <c r="E36" t="s">
+      <c r="G36" t="s">
         <v>118</v>
       </c>
-      <c r="F36" t="s">
+      <c r="H36" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="82">
         <v>29765</v>
       </c>
@@ -20042,17 +20654,23 @@
       <c r="C37" t="s">
         <v>128</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="s">
+        <v>251</v>
+      </c>
+      <c r="E37" s="111" t="s">
+        <v>265</v>
+      </c>
+      <c r="F37">
         <v>8</v>
       </c>
-      <c r="E37" t="s">
+      <c r="G37" t="s">
         <v>129</v>
       </c>
-      <c r="F37" t="s">
+      <c r="H37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="82">
         <v>30186</v>
       </c>
@@ -20062,17 +20680,23 @@
       <c r="C38" t="s">
         <v>128</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="s">
+        <v>233</v>
+      </c>
+      <c r="E38" s="111" t="s">
+        <v>259</v>
+      </c>
+      <c r="F38">
         <v>8</v>
       </c>
-      <c r="E38" t="s">
+      <c r="G38" t="s">
         <v>129</v>
       </c>
-      <c r="F38" t="s">
+      <c r="H38" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="82">
         <v>30286</v>
       </c>
@@ -20082,17 +20706,23 @@
       <c r="C39" t="s">
         <v>108</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="s">
+        <v>244</v>
+      </c>
+      <c r="E39" s="111" t="s">
+        <v>175</v>
+      </c>
+      <c r="F39">
         <v>8</v>
       </c>
-      <c r="E39" t="s">
+      <c r="G39" t="s">
         <v>130</v>
       </c>
-      <c r="F39" t="s">
+      <c r="H39" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="82">
         <v>30532</v>
       </c>
@@ -20102,17 +20732,23 @@
       <c r="C40" t="s">
         <v>131</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="s">
+        <v>252</v>
+      </c>
+      <c r="E40" s="111" t="s">
+        <v>267</v>
+      </c>
+      <c r="F40">
         <v>9</v>
       </c>
-      <c r="E40" t="s">
+      <c r="G40" t="s">
         <v>132</v>
       </c>
-      <c r="F40" t="s">
-        <v>106</v>
+      <c r="H40" t="s">
+        <v>266</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="82">
         <v>31625</v>
       </c>
@@ -20122,17 +20758,23 @@
       <c r="C41" t="s">
         <v>131</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="s">
+        <v>234</v>
+      </c>
+      <c r="E41" s="111" t="s">
+        <v>260</v>
+      </c>
+      <c r="F41">
         <v>9</v>
       </c>
-      <c r="E41" t="s">
+      <c r="G41" t="s">
         <v>133</v>
       </c>
-      <c r="F41" t="s">
-        <v>106</v>
+      <c r="H41" t="s">
+        <v>266</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="82">
         <v>31884</v>
       </c>
@@ -20142,17 +20784,23 @@
       <c r="C42" t="s">
         <v>108</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="111" t="s">
+        <v>268</v>
+      </c>
+      <c r="F42">
         <v>9</v>
       </c>
-      <c r="E42" t="s">
+      <c r="G42" t="s">
         <v>134</v>
       </c>
-      <c r="F42" t="s">
+      <c r="H42" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="82">
         <v>31987</v>
       </c>
@@ -20162,17 +20810,23 @@
       <c r="C43" t="s">
         <v>135</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="s">
+        <v>238</v>
+      </c>
+      <c r="E43" s="111" t="s">
+        <v>269</v>
+      </c>
+      <c r="F43">
         <v>10</v>
       </c>
-      <c r="E43" t="s">
+      <c r="G43" t="s">
         <v>129</v>
       </c>
-      <c r="F43" t="s">
+      <c r="H43" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="82">
         <v>32246</v>
       </c>
@@ -20182,17 +20836,23 @@
       <c r="C44" t="s">
         <v>136</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="s">
+        <v>270</v>
+      </c>
+      <c r="E44" s="111" t="s">
+        <v>275</v>
+      </c>
+      <c r="F44">
         <v>10</v>
       </c>
-      <c r="E44" t="s">
+      <c r="G44" t="s">
         <v>129</v>
       </c>
-      <c r="F44" t="s">
+      <c r="H44" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="82">
         <v>32711</v>
       </c>
@@ -20202,17 +20862,23 @@
       <c r="C45" t="s">
         <v>122</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="s">
+        <v>183</v>
+      </c>
+      <c r="E45" s="111" t="s">
+        <v>276</v>
+      </c>
+      <c r="F45">
         <v>10</v>
       </c>
-      <c r="E45" t="s">
+      <c r="G45" t="s">
         <v>129</v>
       </c>
-      <c r="F45" t="s">
+      <c r="H45" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="82">
         <v>33340</v>
       </c>
@@ -20222,17 +20888,23 @@
       <c r="C46" t="s">
         <v>122</v>
       </c>
-      <c r="D46">
+      <c r="D46" t="s">
+        <v>278</v>
+      </c>
+      <c r="E46" s="111" t="s">
+        <v>277</v>
+      </c>
+      <c r="F46">
         <v>10</v>
       </c>
-      <c r="E46" s="81" t="s">
+      <c r="G46" s="81" t="s">
         <v>130</v>
       </c>
-      <c r="F46" t="s">
+      <c r="H46" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="82">
         <v>33783</v>
       </c>
@@ -20242,17 +20914,23 @@
       <c r="C47" t="s">
         <v>137</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="s">
+        <v>253</v>
+      </c>
+      <c r="E47" s="111" t="s">
+        <v>280</v>
+      </c>
+      <c r="F47">
         <v>11</v>
       </c>
-      <c r="E47" t="s">
+      <c r="G47" t="s">
         <v>130</v>
       </c>
-      <c r="F47" t="s">
+      <c r="H47" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="82">
         <v>34087</v>
       </c>
@@ -20262,17 +20940,23 @@
       <c r="C48" t="s">
         <v>139</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="s">
+        <v>281</v>
+      </c>
+      <c r="E48" s="111" t="s">
+        <v>284</v>
+      </c>
+      <c r="F48">
         <v>11</v>
       </c>
-      <c r="E48" t="s">
+      <c r="G48" t="s">
         <v>138</v>
       </c>
-      <c r="F48" t="s">
+      <c r="H48" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="82">
         <v>34464</v>
       </c>
@@ -20282,17 +20966,23 @@
       <c r="C49" t="s">
         <v>140</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="111" t="s">
+        <v>285</v>
+      </c>
+      <c r="F49">
         <v>12</v>
       </c>
-      <c r="E49" t="s">
+      <c r="G49" t="s">
         <v>141</v>
       </c>
-      <c r="F49" t="s">
+      <c r="H49" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="82">
         <v>34716</v>
       </c>
@@ -20302,17 +20992,23 @@
       <c r="C50" t="s">
         <v>142</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="s">
+        <v>271</v>
+      </c>
+      <c r="E50" s="111" t="s">
+        <v>286</v>
+      </c>
+      <c r="F50">
         <v>12</v>
       </c>
-      <c r="E50" t="s">
+      <c r="G50" t="s">
         <v>143</v>
       </c>
-      <c r="F50" t="s">
+      <c r="H50" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="82">
         <v>35202</v>
       </c>
@@ -20322,17 +21018,23 @@
       <c r="C51" t="s">
         <v>144</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="s">
+        <v>255</v>
+      </c>
+      <c r="E51" s="111" t="s">
+        <v>287</v>
+      </c>
+      <c r="F51">
         <v>13</v>
       </c>
-      <c r="E51" t="s">
+      <c r="G51" t="s">
         <v>145</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="82">
         <v>36089</v>
       </c>
@@ -20342,17 +21044,23 @@
       <c r="C52" t="s">
         <v>146</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="s">
+        <v>256</v>
+      </c>
+      <c r="E52" s="111" t="s">
+        <v>288</v>
+      </c>
+      <c r="F52">
         <v>13</v>
       </c>
-      <c r="E52" t="s">
+      <c r="G52" t="s">
         <v>147</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="82">
         <v>36516</v>
       </c>
@@ -20362,17 +21070,23 @@
       <c r="C53" t="s">
         <v>146</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="s">
+        <v>290</v>
+      </c>
+      <c r="E53" s="111" t="s">
+        <v>289</v>
+      </c>
+      <c r="F53">
         <v>13</v>
       </c>
-      <c r="E53" t="s">
+      <c r="G53" t="s">
         <v>147</v>
       </c>
-      <c r="F53" t="s">
+      <c r="H53" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="82">
         <v>36641</v>
       </c>
@@ -20382,17 +21096,23 @@
       <c r="C54" t="s">
         <v>137</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="s">
+        <v>292</v>
+      </c>
+      <c r="E54" s="111" t="s">
+        <v>261</v>
+      </c>
+      <c r="F54">
         <v>13</v>
       </c>
-      <c r="E54" t="s">
+      <c r="G54" t="s">
         <v>148</v>
       </c>
-      <c r="F54" t="s">
+      <c r="H54" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="82">
         <v>37053</v>
       </c>
@@ -20402,17 +21122,23 @@
       <c r="C55" t="s">
         <v>140</v>
       </c>
-      <c r="D55">
+      <c r="D55" t="s">
+        <v>293</v>
+      </c>
+      <c r="E55" s="111" t="s">
+        <v>262</v>
+      </c>
+      <c r="F55">
         <v>14</v>
       </c>
-      <c r="E55" t="s">
+      <c r="G55" t="s">
         <v>149</v>
       </c>
-      <c r="F55" t="s">
+      <c r="H55" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="82">
         <v>38465</v>
       </c>
@@ -20422,17 +21148,23 @@
       <c r="C56" t="s">
         <v>140</v>
       </c>
-      <c r="D56">
+      <c r="D56" t="s">
+        <v>295</v>
+      </c>
+      <c r="E56" s="111" t="s">
+        <v>248</v>
+      </c>
+      <c r="F56">
         <v>14</v>
       </c>
-      <c r="E56" t="s">
+      <c r="G56" t="s">
         <v>150</v>
       </c>
-      <c r="F56" t="s">
+      <c r="H56" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="82">
         <v>38854</v>
       </c>
@@ -20442,17 +21174,23 @@
       <c r="C57" t="s">
         <v>144</v>
       </c>
-      <c r="D57">
+      <c r="D57" t="s">
+        <v>296</v>
+      </c>
+      <c r="E57" s="111" t="s">
+        <v>263</v>
+      </c>
+      <c r="F57">
         <v>15</v>
       </c>
-      <c r="E57" t="s">
+      <c r="G57" t="s">
         <v>151</v>
       </c>
-      <c r="F57" t="s">
+      <c r="H57" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="82">
         <v>39576</v>
       </c>
@@ -20462,17 +21200,23 @@
       <c r="C58" t="s">
         <v>140</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="s">
+        <v>249</v>
+      </c>
+      <c r="E58" s="111" t="s">
+        <v>297</v>
+      </c>
+      <c r="F58">
         <v>16</v>
       </c>
-      <c r="E58" t="s">
+      <c r="G58" t="s">
         <v>152</v>
       </c>
-      <c r="F58" t="s">
+      <c r="H58" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="82">
         <v>40863</v>
       </c>
@@ -20482,17 +21226,23 @@
       <c r="C59" t="s">
         <v>153</v>
       </c>
-      <c r="D59">
+      <c r="D59" t="s">
+        <v>272</v>
+      </c>
+      <c r="E59" s="111" t="s">
+        <v>298</v>
+      </c>
+      <c r="F59">
         <v>16</v>
       </c>
-      <c r="E59" t="s">
+      <c r="G59" t="s">
         <v>154</v>
       </c>
-      <c r="F59" t="s">
+      <c r="H59" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="82">
         <v>41392</v>
       </c>
@@ -20502,17 +21252,23 @@
       <c r="C60" t="s">
         <v>155</v>
       </c>
-      <c r="D60">
+      <c r="D60" t="s">
+        <v>273</v>
+      </c>
+      <c r="E60" s="111" t="s">
+        <v>299</v>
+      </c>
+      <c r="F60">
         <v>17</v>
       </c>
-      <c r="E60" t="s">
+      <c r="G60" t="s">
         <v>156</v>
       </c>
-      <c r="F60" t="s">
+      <c r="H60" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="82">
         <v>41692</v>
       </c>
@@ -20522,17 +21278,23 @@
       <c r="C61" t="s">
         <v>157</v>
       </c>
-      <c r="D61">
+      <c r="D61" t="s">
+        <v>274</v>
+      </c>
+      <c r="E61" s="111" t="s">
+        <v>300</v>
+      </c>
+      <c r="F61">
         <v>17</v>
       </c>
-      <c r="E61" t="s">
+      <c r="G61" t="s">
         <v>158</v>
       </c>
-      <c r="F61" t="s">
+      <c r="H61" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="82">
         <v>42716</v>
       </c>
@@ -20542,17 +21304,23 @@
       <c r="C62" t="s">
         <v>159</v>
       </c>
-      <c r="D62">
+      <c r="D62" t="s">
+        <v>301</v>
+      </c>
+      <c r="E62" s="111" t="s">
+        <v>302</v>
+      </c>
+      <c r="F62">
         <v>17</v>
       </c>
-      <c r="E62" t="s">
+      <c r="G62" t="s">
         <v>160</v>
       </c>
-      <c r="F62" t="s">
+      <c r="H62" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="82">
         <v>43252</v>
       </c>
@@ -20562,17 +21330,23 @@
       <c r="C63" t="s">
         <v>161</v>
       </c>
-      <c r="D63">
+      <c r="D63" t="s">
+        <v>279</v>
+      </c>
+      <c r="E63" s="111" t="s">
+        <v>303</v>
+      </c>
+      <c r="F63">
         <v>18</v>
       </c>
-      <c r="E63" t="s">
+      <c r="G63" t="s">
         <v>163</v>
       </c>
-      <c r="F63" t="s">
+      <c r="H63" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="82">
         <v>43713</v>
       </c>
@@ -20582,55 +21356,140 @@
       <c r="C64" t="s">
         <v>161</v>
       </c>
-      <c r="D64">
+      <c r="D64" t="s">
+        <v>294</v>
+      </c>
+      <c r="E64" s="111" t="s">
+        <v>291</v>
+      </c>
+      <c r="F64">
         <v>18</v>
       </c>
-      <c r="E64" t="s">
+      <c r="G64" t="s">
         <v>162</v>
       </c>
-      <c r="F64" t="s">
+      <c r="H64" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="82">
         <v>44240</v>
       </c>
-      <c r="B65" s="83">
+      <c r="B65" s="82">
         <v>44856</v>
       </c>
       <c r="C65" t="s">
         <v>164</v>
       </c>
-      <c r="D65">
+      <c r="D65" t="s">
+        <v>282</v>
+      </c>
+      <c r="E65" s="111" t="s">
+        <v>304</v>
+      </c>
+      <c r="F65">
         <v>18</v>
       </c>
-      <c r="E65" t="s">
+      <c r="G65" t="s">
         <v>165</v>
       </c>
-      <c r="F65" t="s">
+      <c r="H65" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="82">
         <v>44856</v>
       </c>
       <c r="C66" t="s">
         <v>166</v>
       </c>
-      <c r="D66">
+      <c r="D66" t="s">
+        <v>283</v>
+      </c>
+      <c r="E66" s="111" t="s">
+        <v>305</v>
+      </c>
+      <c r="F66">
         <v>19</v>
       </c>
-      <c r="E66" t="s">
+      <c r="G66" t="s">
         <v>168</v>
       </c>
-      <c r="F66" t="s">
+      <c r="H66" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D66BF13C-483A-41D8-AD81-16E190447C56}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{F856B41F-E911-46C3-A57F-81442216872C}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{12BCB2F0-5DF3-4055-9D7F-44BA97E755E2}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{D6668578-1EE5-4778-AAE7-050E68B05E71}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{14AE4C93-DC47-4C9F-8BE7-538D7C535233}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{0712E39D-0232-4EBE-ABCD-2E8DBF82F19C}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{4C2A8859-0072-4706-8CCD-941630EBDBFE}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{F6393E6B-B930-487F-802A-69E8C15BDFFB}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{25922FEA-5210-4019-8264-73E8AB6BC8F8}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{F012B9FF-A5E1-4CA8-B5D5-7FDC3573616E}"/>
+    <hyperlink ref="E12" r:id="rId11" xr:uid="{DA459A0B-7B83-43E3-B737-C144D97EBC57}"/>
+    <hyperlink ref="E13" r:id="rId12" xr:uid="{15D2B560-81D8-4E91-8E25-D1C9B7EB0A56}"/>
+    <hyperlink ref="E14" r:id="rId13" xr:uid="{19D53EDE-08AC-4672-BE8C-8BC01170F94D}"/>
+    <hyperlink ref="E15" r:id="rId14" xr:uid="{3AD591DF-6C87-4C59-85CE-0C63C73F4A7F}"/>
+    <hyperlink ref="E16" r:id="rId15" xr:uid="{0CEE4223-6200-47B8-A7E6-7EC7199B1981}"/>
+    <hyperlink ref="E17" r:id="rId16" xr:uid="{02E9F94C-89B4-43F4-87CB-5F158CB307D0}"/>
+    <hyperlink ref="E18" r:id="rId17" xr:uid="{7024846A-376D-4A08-9608-C6C9A12DF6F5}"/>
+    <hyperlink ref="E19" r:id="rId18" xr:uid="{7C98E1D9-C7B4-4970-961E-81E3EB972DDE}"/>
+    <hyperlink ref="E20" r:id="rId19" xr:uid="{DFD06C3A-4FA9-4B54-ABB6-E610AF0B36A9}"/>
+    <hyperlink ref="E21" r:id="rId20" xr:uid="{EE9AD55C-93B4-4CB9-B637-95A8113CC915}"/>
+    <hyperlink ref="E22" r:id="rId21" xr:uid="{743D1254-FFA5-4682-A946-FBB42A046D90}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{440B9E75-00C4-4E98-9903-00269C1A14E1}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{6D6574AD-6D95-4C71-9415-53ABB98353A7}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{298AD0A7-4CA3-4C41-B5D1-D4D866127FD4}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{D5FEBC0D-89CB-47A3-97E3-2F4513FCA108}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{1C6D51E6-416D-4262-B795-778266044E4F}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{C2AFD6CD-BCA9-46FF-A8DD-5C85ECE1059B}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{B7753F55-BE5D-4133-99FF-BC0A58DFCE7B}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{B1AA4F5B-498F-482F-8A9C-328AE7767354}"/>
+    <hyperlink ref="E31" r:id="rId30" xr:uid="{D39C54E7-D0FA-47F2-A8A4-2B7689D64DD1}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{2118C62E-025E-4B4C-BF40-84940FA47C6F}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{4A5086B5-003D-4367-8AB3-204940275459}"/>
+    <hyperlink ref="E34" r:id="rId33" xr:uid="{2E77EDD8-E203-4203-BF6E-89D3418BCCD5}"/>
+    <hyperlink ref="E35" r:id="rId34" xr:uid="{365C9CBA-70BE-4BD0-875B-15A6FB85DCFA}"/>
+    <hyperlink ref="E36" r:id="rId35" xr:uid="{BCF24484-0388-404C-B297-8246AEDF8E40}"/>
+    <hyperlink ref="E37" r:id="rId36" xr:uid="{7C360199-3EA9-4A2A-8CD1-C7F7D655EBBC}"/>
+    <hyperlink ref="E38" r:id="rId37" xr:uid="{45D535C5-DED2-44F2-9E66-BA17BCC0A66E}"/>
+    <hyperlink ref="E39" r:id="rId38" xr:uid="{CA50CBF7-2D32-4DE4-92D5-F22A3C6E0FA2}"/>
+    <hyperlink ref="E40" r:id="rId39" xr:uid="{978209CD-75B2-44B0-B917-CD120FFE58E4}"/>
+    <hyperlink ref="E41" r:id="rId40" xr:uid="{58304222-DA43-421C-A778-3E7FD2B12E94}"/>
+    <hyperlink ref="E42" r:id="rId41" xr:uid="{0797F7C4-3782-42AD-91BD-96F8C72B00D2}"/>
+    <hyperlink ref="E43" r:id="rId42" xr:uid="{B9E83DFF-8E6A-4ECC-9C9A-DC8F6B559F75}"/>
+    <hyperlink ref="E44" r:id="rId43" xr:uid="{4285979A-C1F6-417F-A2E6-02BEF0206579}"/>
+    <hyperlink ref="E45" r:id="rId44" xr:uid="{DF0DD79F-0A83-4070-99B5-F89B35B00CE7}"/>
+    <hyperlink ref="E46" r:id="rId45" xr:uid="{8F1C2101-1EE6-4E43-9435-324151D5FC0F}"/>
+    <hyperlink ref="E47" r:id="rId46" xr:uid="{36986592-5063-4F57-8186-DFF6F0E510AC}"/>
+    <hyperlink ref="E48" r:id="rId47" xr:uid="{A2C0A21E-32B5-4223-9948-8D6D3F5D3BF0}"/>
+    <hyperlink ref="E49" r:id="rId48" xr:uid="{37C74CF5-CE40-4312-BD62-C7D58CBF511D}"/>
+    <hyperlink ref="E50" r:id="rId49" xr:uid="{0BA90E9C-DFC8-4A24-A8AD-9D4C9266F49C}"/>
+    <hyperlink ref="E51" r:id="rId50" xr:uid="{2981DBC6-6DF0-4109-82D3-2EF1EF96287D}"/>
+    <hyperlink ref="E52" r:id="rId51" xr:uid="{ACB3EBD6-B3A4-45CF-AE58-229629249748}"/>
+    <hyperlink ref="E53" r:id="rId52" xr:uid="{BF00807F-00A4-4677-B185-57A3F9924BD9}"/>
+    <hyperlink ref="E54" r:id="rId53" xr:uid="{CADC2F01-116F-403B-AD26-05E4EC3C2817}"/>
+    <hyperlink ref="E55" r:id="rId54" xr:uid="{3A42F3D0-6E2A-4265-90CD-E949CA1AEADA}"/>
+    <hyperlink ref="E56" r:id="rId55" xr:uid="{8160E50D-4014-425B-9F04-022F9123334A}"/>
+    <hyperlink ref="E57" r:id="rId56" xr:uid="{BC5DFBF7-01F5-4A83-B810-8CB2BAAA1FDD}"/>
+    <hyperlink ref="E58" r:id="rId57" xr:uid="{6A10AE00-BDB9-4D16-BB3B-E0F539461EAF}"/>
+    <hyperlink ref="E59" r:id="rId58" xr:uid="{52236FB6-4AAA-44D2-AEB4-8C0AF09C240C}"/>
+    <hyperlink ref="E60" r:id="rId59" xr:uid="{D706343F-8993-4E65-BFD7-7A7371DFB773}"/>
+    <hyperlink ref="E61" r:id="rId60" xr:uid="{5CC36BF8-316F-4682-A2EA-4D384F587BE1}"/>
+    <hyperlink ref="E62" r:id="rId61" xr:uid="{469A71A5-DFC2-454C-96FD-1AF036214FF9}"/>
+    <hyperlink ref="E63" r:id="rId62" xr:uid="{1C5959A2-CC8D-4957-B94A-5C1889E4A59D}"/>
+    <hyperlink ref="E64" r:id="rId63" xr:uid="{E3A3C50F-2117-42DC-887A-62D53C4CD3D5}"/>
+    <hyperlink ref="E65" r:id="rId64" xr:uid="{D3583B41-8C7A-421C-9106-DE91B53C8EA1}"/>
+    <hyperlink ref="E66" r:id="rId65" xr:uid="{923A97DA-9B17-4D08-AD83-22D3ABF9D90A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>